<commit_message>
Mets à jour la table de distribution des ressources
</commit_message>
<xml_diff>
--- a/Schémas.xlsx
+++ b/Schémas.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicolas\Dropbox\ECO+\TEAM Mouchi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicolas\Documents\GitHub\L3T\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735"/>
   </bookViews>
   <sheets>
     <sheet name="Ressources" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="95">
   <si>
     <t>Agriculture</t>
   </si>
@@ -307,13 +307,16 @@
   </si>
   <si>
     <t>armes</t>
+  </si>
+  <si>
+    <t>Arctique</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -336,13 +339,38 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -382,7 +410,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -414,10 +442,6 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -435,6 +459,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -747,38 +789,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:T42"/>
+  <dimension ref="B2:U42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="3" max="10" width="12" customWidth="1"/>
+    <col min="3" max="11" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B3" s="4"/>
       <c r="C3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="26" t="s">
         <v>7</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="26" t="s">
         <v>9</v>
       </c>
       <c r="H3" s="5" t="s">
@@ -790,20 +832,23 @@
       <c r="J3" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="L3" s="19" t="s">
+      <c r="K3" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="M3" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="M3" s="18"/>
-    </row>
-    <row r="4" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="N3" s="16"/>
+    </row>
+    <row r="4" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="6">
-        <v>0.7</v>
+        <v>0.8</v>
       </c>
       <c r="D4" s="6">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
@@ -815,37 +860,41 @@
         <v>0.3</v>
       </c>
       <c r="J4" s="5"/>
-      <c r="L4" t="s">
+      <c r="K4" s="6"/>
+      <c r="M4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B5" s="4" t="s">
+    <row r="5" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B5" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="21">
+        <v>0.15</v>
+      </c>
+      <c r="D5" s="21">
+        <v>0.2</v>
+      </c>
+      <c r="E5" s="21">
         <v>0.25</v>
       </c>
-      <c r="D5" s="6">
-        <v>0.4</v>
-      </c>
-      <c r="E5" s="6">
-        <v>0.5</v>
-      </c>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6">
+      <c r="F5" s="21"/>
+      <c r="G5" s="21"/>
+      <c r="H5" s="21"/>
+      <c r="I5" s="21">
         <v>0.9</v>
       </c>
-      <c r="J5" s="5"/>
-    </row>
-    <row r="6" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="J5" s="22"/>
+      <c r="K5" s="21">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="6" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="6">
-        <v>0.2</v>
+        <v>0.17499999999999999</v>
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
@@ -856,64 +905,70 @@
       <c r="H6" s="6"/>
       <c r="I6" s="5"/>
       <c r="J6" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B7" s="4" t="s">
+        <v>0.6</v>
+      </c>
+      <c r="K6" s="6">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="7" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B7" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6">
-        <v>0.2</v>
-      </c>
-      <c r="E7" s="6">
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21">
         <v>0.7</v>
       </c>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6">
-        <v>0.4</v>
-      </c>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-    </row>
-    <row r="8" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="F7" s="21"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="21">
+        <v>0.3</v>
+      </c>
+      <c r="I7" s="22"/>
+      <c r="J7" s="22"/>
+      <c r="K7" s="21"/>
+      <c r="M7" s="27"/>
+    </row>
+    <row r="8" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="6">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="E8" s="6">
-        <v>0.25</v>
+        <v>0.125</v>
       </c>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
       <c r="H8" s="6">
-        <v>0.65</v>
+        <v>0.7</v>
       </c>
       <c r="I8" s="5"/>
       <c r="J8" s="6">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="9" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B9" s="4" t="s">
+        <v>0.25</v>
+      </c>
+      <c r="K8" s="6">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="9" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B9" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="21"/>
+      <c r="D9" s="21">
         <v>0.35</v>
       </c>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-      <c r="L9" s="8"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="22"/>
+      <c r="J9" s="22"/>
+      <c r="K9" s="21"/>
       <c r="M9" s="8"/>
       <c r="N9" s="8"/>
       <c r="O9" s="8"/>
@@ -922,18 +977,19 @@
       <c r="R9" s="8"/>
       <c r="S9" s="8"/>
       <c r="T9" s="8"/>
-    </row>
-    <row r="10" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U9" s="8"/>
+    </row>
+    <row r="10" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B10" s="8"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="15"/>
-      <c r="J10" s="15"/>
-      <c r="L10" s="8"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="13"/>
       <c r="M10" s="8"/>
       <c r="N10" s="8"/>
       <c r="O10" s="8"/>
@@ -942,12 +998,12 @@
       <c r="R10" s="8"/>
       <c r="S10" s="8"/>
       <c r="T10" s="8"/>
-    </row>
-    <row r="11" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U10" s="8"/>
+    </row>
+    <row r="11" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>19</v>
       </c>
-      <c r="L11" s="8"/>
       <c r="M11" s="8"/>
       <c r="N11" s="8"/>
       <c r="O11" s="8"/>
@@ -956,16 +1012,17 @@
       <c r="R11" s="8"/>
       <c r="S11" s="8"/>
       <c r="T11" s="8"/>
-    </row>
-    <row r="12" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U11" s="8"/>
+    </row>
+    <row r="12" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B12" s="4"/>
       <c r="C12" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="E12" s="26" t="s">
         <v>7</v>
       </c>
       <c r="F12" s="5" t="s">
@@ -983,32 +1040,35 @@
       <c r="J12" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="L12" s="15"/>
-      <c r="M12" s="15"/>
-      <c r="N12" s="15"/>
-      <c r="O12" s="15"/>
-      <c r="P12" s="15"/>
-      <c r="Q12" s="15"/>
-      <c r="R12" s="15"/>
-      <c r="S12" s="15"/>
-      <c r="T12" s="8"/>
-    </row>
-    <row r="13" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="K12" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="M12" s="13"/>
+      <c r="N12" s="13"/>
+      <c r="O12" s="13"/>
+      <c r="P12" s="13"/>
+      <c r="Q12" s="13"/>
+      <c r="R12" s="13"/>
+      <c r="S12" s="13"/>
+      <c r="T12" s="13"/>
+      <c r="U12" s="8"/>
+    </row>
+    <row r="13" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C13" s="7">
         <f>C4/(1-C$19)</f>
-        <v>0.79275198187995466</v>
+        <v>0.93050305321314342</v>
       </c>
       <c r="D13" s="7">
-        <f t="shared" ref="D13:I13" si="0">D4/(1-D$19)</f>
-        <v>0.24752475247524752</v>
+        <f>D4/(1-D$19)</f>
+        <v>0.12303149606299214</v>
       </c>
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
       <c r="G13" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="D13:I13" si="0">G4/(1-G$19)</f>
         <v>1</v>
       </c>
       <c r="H13" s="7"/>
@@ -1017,7 +1077,7 @@
         <v>0.32258064516129031</v>
       </c>
       <c r="J13" s="7"/>
-      <c r="L13" s="8"/>
+      <c r="K13" s="7"/>
       <c r="M13" s="8"/>
       <c r="N13" s="8"/>
       <c r="O13" s="8"/>
@@ -1026,32 +1086,36 @@
       <c r="R13" s="8"/>
       <c r="S13" s="8"/>
       <c r="T13" s="8"/>
-    </row>
-    <row r="14" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B14" s="4" t="s">
+      <c r="U13" s="8"/>
+    </row>
+    <row r="14" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B14" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C14" s="7">
+      <c r="C14" s="23">
         <f>C5/(1-C$19)</f>
-        <v>0.28312570781426954</v>
-      </c>
-      <c r="D14" s="7">
+        <v>0.17446932247746438</v>
+      </c>
+      <c r="D14" s="23">
         <f>D5/(1-D$19)</f>
-        <v>0.49504950495049505</v>
-      </c>
-      <c r="E14" s="7">
+        <v>0.24606299212598429</v>
+      </c>
+      <c r="E14" s="23">
         <f>E5/(1-E$19)</f>
-        <v>0.56338028169014087</v>
-      </c>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7">
+        <v>0.31128404669260701</v>
+      </c>
+      <c r="F14" s="23"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="23"/>
+      <c r="I14" s="23">
         <f t="shared" ref="I14" si="1">I5/(1-I$19)</f>
         <v>0.96774193548387089</v>
       </c>
-      <c r="J14" s="7"/>
-      <c r="L14" s="8"/>
+      <c r="J14" s="23"/>
+      <c r="K14" s="23">
+        <f t="shared" ref="J14:K15" si="2">K5/(1-K$19)</f>
+        <v>0.1801801801801802</v>
+      </c>
       <c r="M14" s="8"/>
       <c r="N14" s="8"/>
       <c r="O14" s="8"/>
@@ -1060,14 +1124,15 @@
       <c r="R14" s="8"/>
       <c r="S14" s="8"/>
       <c r="T14" s="8"/>
-    </row>
-    <row r="15" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U14" s="8"/>
+    </row>
+    <row r="15" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C15" s="7">
         <f>C6/(1-C$19)</f>
-        <v>0.22650056625141565</v>
+        <v>0.2035475428903751</v>
       </c>
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
@@ -1079,41 +1144,42 @@
       <c r="H15" s="7"/>
       <c r="I15" s="7"/>
       <c r="J15" s="7">
-        <f t="shared" ref="J15" si="2">J6/(1-J$19)</f>
-        <v>1</v>
-      </c>
-      <c r="L15" s="15"/>
-      <c r="M15" s="15"/>
-      <c r="N15" s="15"/>
-      <c r="O15" s="15"/>
-      <c r="P15" s="15"/>
-      <c r="Q15" s="15"/>
-      <c r="R15" s="15"/>
-      <c r="S15" s="15"/>
-      <c r="T15" s="8"/>
-    </row>
-    <row r="16" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B16" s="4" t="s">
+        <f t="shared" si="2"/>
+        <v>0.85714285714285721</v>
+      </c>
+      <c r="K15" s="7">
+        <f>K6/(1-K$19)</f>
+        <v>0.86486486486486491</v>
+      </c>
+      <c r="M15" s="13"/>
+      <c r="N15" s="13"/>
+      <c r="O15" s="13"/>
+      <c r="P15" s="13"/>
+      <c r="Q15" s="13"/>
+      <c r="R15" s="13"/>
+      <c r="S15" s="13"/>
+      <c r="T15" s="13"/>
+      <c r="U15" s="8"/>
+    </row>
+    <row r="16" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B16" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7">
-        <f>D7/(1-D$19)</f>
-        <v>0.24752475247524752</v>
-      </c>
-      <c r="E16" s="7">
+      <c r="C16" s="23"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="23">
         <f>E7/(1-E$19)</f>
-        <v>0.78873239436619713</v>
-      </c>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7">
+        <v>0.87159533073929962</v>
+      </c>
+      <c r="F16" s="23"/>
+      <c r="G16" s="23"/>
+      <c r="H16" s="23">
         <f>H7/(1-H$19)</f>
-        <v>0.50632911392405067</v>
-      </c>
-      <c r="I16" s="7"/>
-      <c r="J16" s="7"/>
-      <c r="L16" s="8"/>
+        <v>0.37974683544303794</v>
+      </c>
+      <c r="I16" s="23"/>
+      <c r="J16" s="23"/>
+      <c r="K16" s="23"/>
       <c r="M16" s="8"/>
       <c r="N16" s="8"/>
       <c r="O16" s="8"/>
@@ -1122,32 +1188,36 @@
       <c r="R16" s="8"/>
       <c r="S16" s="8"/>
       <c r="T16" s="8"/>
-    </row>
-    <row r="17" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U16" s="8"/>
+    </row>
+    <row r="17" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B17" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C17" s="7"/>
       <c r="D17" s="7">
         <f>D8/(1-D$19)</f>
-        <v>0.61881188118811881</v>
+        <v>0.73818897637795278</v>
       </c>
       <c r="E17" s="7">
         <f>E8/(1-E$19)</f>
-        <v>0.28169014084507044</v>
+        <v>0.1556420233463035</v>
       </c>
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
       <c r="H17" s="7">
         <f>H8/(1-H$19)</f>
-        <v>0.82278481012658222</v>
+        <v>0.88607594936708856</v>
       </c>
       <c r="I17" s="7"/>
       <c r="J17" s="7">
-        <f t="shared" ref="J17" si="3">J8/(1-J$19)</f>
-        <v>0.2</v>
-      </c>
-      <c r="L17" s="8"/>
+        <f t="shared" ref="J17:K17" si="3">J8/(1-J$19)</f>
+        <v>0.35714285714285715</v>
+      </c>
+      <c r="K17" s="7">
+        <f t="shared" si="3"/>
+        <v>0.1801801801801802</v>
+      </c>
       <c r="M17" s="8"/>
       <c r="N17" s="8"/>
       <c r="O17" s="8"/>
@@ -1156,23 +1226,24 @@
       <c r="R17" s="8"/>
       <c r="S17" s="8"/>
       <c r="T17" s="8"/>
-    </row>
-    <row r="18" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B18" s="4" t="s">
+      <c r="U17" s="8"/>
+    </row>
+    <row r="18" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B18" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="C18" s="7">
-        <f>C9/(1-C$19)</f>
-        <v>0.39637599093997733</v>
-      </c>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
-      <c r="J18" s="7"/>
-      <c r="L18" s="8"/>
+      <c r="C18" s="23"/>
+      <c r="D18" s="23">
+        <f>D9/(1-D$19)</f>
+        <v>0.43061023622047245</v>
+      </c>
+      <c r="E18" s="23"/>
+      <c r="F18" s="23"/>
+      <c r="G18" s="23"/>
+      <c r="H18" s="23"/>
+      <c r="I18" s="23"/>
+      <c r="J18" s="23"/>
+      <c r="K18" s="23"/>
       <c r="M18" s="8"/>
       <c r="N18" s="8"/>
       <c r="O18" s="8"/>
@@ -1181,22 +1252,23 @@
       <c r="R18" s="8"/>
       <c r="S18" s="8"/>
       <c r="T18" s="8"/>
-    </row>
-    <row r="19" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U18" s="8"/>
+    </row>
+    <row r="19" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B19" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C19" s="11">
         <f>(1-C4)*(1-C5)*(1-C6)*(1-C7)*(1-C8)*(1-C9)</f>
-        <v>0.11700000000000003</v>
+        <v>0.14024999999999996</v>
       </c>
       <c r="D19" s="11">
-        <f t="shared" ref="D19:J19" si="4">(1-D4)*(1-D5)*(1-D6)*(1-D7)*(1-D8)*(1-D9)</f>
-        <v>0.192</v>
+        <f>(1-D4)*(1-D5)*(1-D6)*(1-D7)*(1-D8)*(1-D9)</f>
+        <v>0.18720000000000003</v>
       </c>
       <c r="E19" s="11">
-        <f t="shared" si="4"/>
-        <v>0.11250000000000002</v>
+        <f t="shared" ref="D19:K19" si="4">(1-E4)*(1-E5)*(1-E6)*(1-E7)*(1-E8)*(1-E9)</f>
+        <v>0.19687500000000002</v>
       </c>
       <c r="F19" s="11">
         <f t="shared" si="4"/>
@@ -1208,7 +1280,7 @@
       </c>
       <c r="H19" s="11">
         <f t="shared" si="4"/>
-        <v>0.21</v>
+        <v>0.21000000000000002</v>
       </c>
       <c r="I19" s="11">
         <f t="shared" si="4"/>
@@ -1216,54 +1288,62 @@
       </c>
       <c r="J19" s="11">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="L19" t="s">
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="K19" s="11">
+        <f t="shared" si="4"/>
+        <v>0.30625000000000002</v>
+      </c>
+      <c r="M19" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B20" s="13" t="s">
+    <row r="20" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B20" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="C20" s="14">
+      <c r="C20" s="25">
         <f>SUM(C13:C18)</f>
-        <v>1.6987542468856172</v>
-      </c>
-      <c r="D20" s="14">
+        <v>1.3085199185809828</v>
+      </c>
+      <c r="D20" s="25">
         <f t="shared" ref="D20:I20" si="5">SUM(D13:D18)</f>
-        <v>1.608910891089109</v>
-      </c>
-      <c r="E20" s="14">
+        <v>1.5378937007874016</v>
+      </c>
+      <c r="E20" s="25">
         <f t="shared" si="5"/>
-        <v>1.6338028169014085</v>
-      </c>
-      <c r="F20" s="14">
+        <v>1.3385214007782102</v>
+      </c>
+      <c r="F20" s="25">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="G20" s="14">
+      <c r="G20" s="25">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="H20" s="14">
+      <c r="H20" s="25">
         <f t="shared" si="5"/>
-        <v>1.3291139240506329</v>
-      </c>
-      <c r="I20" s="14">
+        <v>1.2658227848101264</v>
+      </c>
+      <c r="I20" s="25">
         <f t="shared" si="5"/>
         <v>1.2903225806451613</v>
       </c>
-      <c r="J20" s="14">
+      <c r="J20" s="25">
         <f>SUM(J13:J18)</f>
-        <v>1.2</v>
-      </c>
-      <c r="L20" t="s">
+        <v>1.2142857142857144</v>
+      </c>
+      <c r="K20" s="25">
+        <f>SUM(K13:K18)</f>
+        <v>1.2252252252252251</v>
+      </c>
+      <c r="M20" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B21" s="17"/>
+    <row r="21" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B21" s="15"/>
       <c r="C21" s="12"/>
       <c r="D21" s="12"/>
       <c r="E21" s="12"/>
@@ -1272,8 +1352,9 @@
       <c r="H21" s="12"/>
       <c r="I21" s="12"/>
       <c r="J21" s="12"/>
-    </row>
-    <row r="22" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="K21" s="12"/>
+    </row>
+    <row r="22" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>17</v>
       </c>
@@ -1285,8 +1366,9 @@
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
       <c r="J22" s="3"/>
-    </row>
-    <row r="23" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="K22" s="3"/>
+    </row>
+    <row r="23" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B23" s="4"/>
       <c r="C23" s="5" t="s">
         <v>5</v>
@@ -1312,23 +1394,26 @@
       <c r="J23" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="24" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="K23" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="24" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C24" s="6">
         <f>C4</f>
-        <v>0.7</v>
+        <v>0.8</v>
       </c>
       <c r="D24" s="6">
-        <f t="shared" ref="D24:G24" si="6">D4</f>
-        <v>0.2</v>
+        <f>D4</f>
+        <v>0.1</v>
       </c>
       <c r="E24" s="6"/>
       <c r="F24" s="6"/>
       <c r="G24" s="6">
-        <f t="shared" si="6"/>
+        <f>G4</f>
         <v>1</v>
       </c>
       <c r="H24" s="6"/>
@@ -1337,44 +1422,49 @@
         <v>0.3</v>
       </c>
       <c r="J24" s="6"/>
-    </row>
-    <row r="25" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B25" s="4" t="s">
+      <c r="K24" s="6"/>
+    </row>
+    <row r="25" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B25" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C25" s="6">
-        <f t="shared" ref="C25:H28" si="7">C5</f>
+      <c r="C25" s="21">
+        <f>C5</f>
+        <v>0.15</v>
+      </c>
+      <c r="D25" s="21">
+        <f>D5</f>
+        <v>0.2</v>
+      </c>
+      <c r="E25" s="21">
+        <f>E5</f>
         <v>0.25</v>
       </c>
-      <c r="D25" s="6">
-        <f t="shared" si="7"/>
-        <v>0.4</v>
-      </c>
-      <c r="E25" s="6">
-        <f t="shared" si="7"/>
-        <v>0.5</v>
-      </c>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
-      <c r="I25" s="6">
+      <c r="F25" s="21"/>
+      <c r="G25" s="21"/>
+      <c r="H25" s="21"/>
+      <c r="I25" s="21">
         <f>I5</f>
         <v>0.9</v>
       </c>
-      <c r="J25" s="6"/>
-    </row>
-    <row r="26" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="J25" s="21"/>
+      <c r="K25" s="21">
+        <f>K5</f>
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="26" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B26" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C26" s="6">
-        <f t="shared" si="7"/>
-        <v>0.2</v>
+        <f>C6</f>
+        <v>0.17499999999999999</v>
       </c>
       <c r="D26" s="6"/>
       <c r="E26" s="6"/>
       <c r="F26" s="6">
-        <f t="shared" si="7"/>
+        <f>F6</f>
         <v>1</v>
       </c>
       <c r="G26" s="6"/>
@@ -1382,97 +1472,107 @@
       <c r="I26" s="6"/>
       <c r="J26" s="6">
         <f>J6</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B27" s="4" t="s">
+        <v>0.6</v>
+      </c>
+      <c r="K26" s="6">
+        <f>K6</f>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="27" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B27" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6">
-        <f t="shared" si="7"/>
-        <v>0.2</v>
-      </c>
-      <c r="E27" s="6">
-        <f t="shared" si="7"/>
+      <c r="C27" s="21"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="21">
+        <f>E7</f>
         <v>0.7</v>
       </c>
-      <c r="F27" s="6"/>
-      <c r="G27" s="6"/>
-      <c r="H27" s="6">
-        <f t="shared" si="7"/>
-        <v>0.4</v>
-      </c>
-      <c r="I27" s="6"/>
-      <c r="J27" s="6"/>
-    </row>
-    <row r="28" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="F27" s="21"/>
+      <c r="G27" s="21"/>
+      <c r="H27" s="21">
+        <f>H7</f>
+        <v>0.3</v>
+      </c>
+      <c r="I27" s="21"/>
+      <c r="J27" s="21"/>
+      <c r="K27" s="21"/>
+    </row>
+    <row r="28" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B28" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C28" s="6"/>
       <c r="D28" s="6">
-        <f t="shared" si="7"/>
-        <v>0.5</v>
+        <f>D8</f>
+        <v>0.6</v>
       </c>
       <c r="E28" s="6">
-        <f t="shared" si="7"/>
-        <v>0.25</v>
+        <f>E8</f>
+        <v>0.125</v>
       </c>
       <c r="F28" s="6"/>
       <c r="G28" s="6"/>
       <c r="H28" s="6">
-        <f t="shared" si="7"/>
-        <v>0.65</v>
+        <f>H8</f>
+        <v>0.7</v>
       </c>
       <c r="I28" s="6"/>
       <c r="J28" s="6">
         <f>J8</f>
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="29" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B29" s="4" t="s">
+        <v>0.25</v>
+      </c>
+      <c r="K28" s="6">
+        <f>K8</f>
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="29" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B29" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="C29" s="6">
-        <v>0.5</v>
-      </c>
-      <c r="D29" s="6">
-        <v>0.5</v>
-      </c>
-      <c r="E29" s="6">
-        <v>0.5</v>
-      </c>
-      <c r="F29" s="6">
-        <v>0.5</v>
-      </c>
-      <c r="G29" s="6">
-        <v>0.5</v>
-      </c>
-      <c r="H29" s="6">
-        <v>0.5</v>
-      </c>
-      <c r="I29" s="6">
-        <v>0.5</v>
-      </c>
-      <c r="J29" s="6">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="30" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="C29" s="21">
+        <v>0.35</v>
+      </c>
+      <c r="D29" s="21">
+        <v>0.35</v>
+      </c>
+      <c r="E29" s="21">
+        <v>0.35</v>
+      </c>
+      <c r="F29" s="21">
+        <v>0.35</v>
+      </c>
+      <c r="G29" s="21">
+        <v>0.35</v>
+      </c>
+      <c r="H29" s="21">
+        <v>0.35</v>
+      </c>
+      <c r="I29" s="21">
+        <v>0.35</v>
+      </c>
+      <c r="J29" s="21">
+        <v>0.35</v>
+      </c>
+      <c r="K29" s="21">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="30" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B30" s="8"/>
-      <c r="C30" s="16"/>
-      <c r="D30" s="16"/>
-      <c r="E30" s="16"/>
-      <c r="F30" s="16"/>
-      <c r="G30" s="16"/>
-      <c r="H30" s="16"/>
-      <c r="I30" s="16"/>
-      <c r="J30" s="16"/>
-    </row>
-    <row r="31" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="C30" s="14"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="14"/>
+      <c r="F30" s="14"/>
+      <c r="G30" s="14"/>
+      <c r="H30" s="14"/>
+      <c r="I30" s="14"/>
+      <c r="J30" s="14"/>
+      <c r="K30" s="14"/>
+    </row>
+    <row r="31" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>16</v>
       </c>
@@ -1484,8 +1584,9 @@
       <c r="H31" s="9"/>
       <c r="I31" s="9"/>
       <c r="J31" s="9"/>
-    </row>
-    <row r="32" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="K31" s="9"/>
+    </row>
+    <row r="32" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B32" s="4"/>
       <c r="C32" s="5" t="s">
         <v>5</v>
@@ -1511,73 +1612,75 @@
       <c r="J32" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="K32" s="1"/>
-    </row>
-    <row r="33" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="K32" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="L32" s="1"/>
+    </row>
+    <row r="33" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B33" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C33" s="7">
         <f>C24/(1-C$39)</f>
-        <v>0.76923076923076927</v>
+        <v>0.88024536839644063</v>
       </c>
       <c r="D33" s="7">
-        <f t="shared" ref="D33:I33" si="8">D24/(1-D$39)</f>
-        <v>0.22123893805309736</v>
+        <f t="shared" ref="D33:I33" si="6">D24/(1-D$39)</f>
+        <v>0.12303149606299214</v>
       </c>
       <c r="E33" s="7"/>
       <c r="F33" s="7"/>
       <c r="G33" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="H33" s="7"/>
       <c r="I33" s="7">
-        <f t="shared" si="8"/>
-        <v>0.31088082901554404</v>
+        <f t="shared" si="6"/>
+        <v>0.31430068098480879</v>
       </c>
       <c r="J33" s="7"/>
-      <c r="K33" s="1"/>
-    </row>
-    <row r="34" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B34" s="4" t="s">
+      <c r="K33" s="7"/>
+      <c r="L33" s="1"/>
+    </row>
+    <row r="34" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B34" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C34" s="7">
+      <c r="C34" s="23">
         <f>C25/(1-C$39)</f>
-        <v>0.27472527472527475</v>
-      </c>
-      <c r="D34" s="7">
+        <v>0.1650460065743326</v>
+      </c>
+      <c r="D34" s="23">
         <f>D25/(1-D$39)</f>
-        <v>0.44247787610619471</v>
-      </c>
-      <c r="E34" s="7">
+        <v>0.24606299212598429</v>
+      </c>
+      <c r="E34" s="23">
         <f>E25/(1-E$39)</f>
-        <v>0.5298013245033113</v>
-      </c>
-      <c r="F34" s="7">
-        <f t="shared" ref="F34:J34" si="9">F25/(1-F$39)</f>
-        <v>0</v>
-      </c>
-      <c r="G34" s="7"/>
-      <c r="H34" s="7"/>
-      <c r="I34" s="7">
-        <f t="shared" si="9"/>
-        <v>0.93264248704663222</v>
-      </c>
-      <c r="J34" s="7">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="K34" s="1"/>
-    </row>
-    <row r="35" spans="2:12" x14ac:dyDescent="0.25">
+        <v>0.28668697366063428</v>
+      </c>
+      <c r="F34" s="23"/>
+      <c r="G34" s="23"/>
+      <c r="H34" s="23"/>
+      <c r="I34" s="23">
+        <f t="shared" ref="F34:J34" si="7">I25/(1-I$39)</f>
+        <v>0.94290204295442637</v>
+      </c>
+      <c r="J34" s="23"/>
+      <c r="K34" s="23">
+        <f t="shared" ref="K34" si="8">K25/(1-K$39)</f>
+        <v>0.15606710885680844</v>
+      </c>
+      <c r="L34" s="1"/>
+    </row>
+    <row r="35" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B35" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C35" s="7">
         <f>C26/(1-C$39)</f>
-        <v>0.2197802197802198</v>
+        <v>0.19255367433672135</v>
       </c>
       <c r="D35" s="7"/>
       <c r="E35" s="7"/>
@@ -1589,183 +1692,198 @@
       <c r="H35" s="7"/>
       <c r="I35" s="7"/>
       <c r="J35" s="7">
-        <f t="shared" ref="J35" si="10">J26/(1-J$39)</f>
-        <v>1</v>
-      </c>
-      <c r="K35" s="1"/>
-    </row>
-    <row r="36" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B36" s="4" t="s">
+        <f t="shared" ref="J35:K35" si="9">J26/(1-J$39)</f>
+        <v>0.74534161490683237</v>
+      </c>
+      <c r="K35" s="7">
+        <f t="shared" si="9"/>
+        <v>0.7491221225126804</v>
+      </c>
+      <c r="L35" s="1"/>
+    </row>
+    <row r="36" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B36" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="C36" s="7"/>
-      <c r="D36" s="7">
-        <f t="shared" ref="D36:E38" si="11">D27/(1-D$39)</f>
-        <v>0.22123893805309736</v>
-      </c>
-      <c r="E36" s="7">
-        <f t="shared" si="11"/>
-        <v>0.74172185430463577</v>
-      </c>
-      <c r="F36" s="7"/>
-      <c r="G36" s="7"/>
-      <c r="H36" s="7">
+      <c r="C36" s="23"/>
+      <c r="D36" s="23"/>
+      <c r="E36" s="23">
+        <f>E27/(1-E$39)</f>
+        <v>0.80272352624977594</v>
+      </c>
+      <c r="F36" s="23"/>
+      <c r="G36" s="23"/>
+      <c r="H36" s="23">
         <f>H27/(1-H$39)</f>
-        <v>0.44692737430167601</v>
-      </c>
-      <c r="I36" s="7"/>
-      <c r="J36" s="7"/>
-      <c r="K36" s="1"/>
-    </row>
-    <row r="37" spans="2:12" x14ac:dyDescent="0.25">
+        <v>0.34742327735958312</v>
+      </c>
+      <c r="I36" s="23"/>
+      <c r="J36" s="23"/>
+      <c r="K36" s="23"/>
+      <c r="L36" s="1"/>
+    </row>
+    <row r="37" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B37" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C37" s="7"/>
       <c r="D37" s="7">
-        <f t="shared" si="11"/>
-        <v>0.55309734513274333</v>
+        <f>D28/(1-D$39)</f>
+        <v>0.73818897637795278</v>
       </c>
       <c r="E37" s="7">
-        <f t="shared" si="11"/>
-        <v>0.26490066225165565</v>
+        <f>E28/(1-E$39)</f>
+        <v>0.14334348683031714</v>
       </c>
       <c r="F37" s="7"/>
       <c r="G37" s="7"/>
       <c r="H37" s="7">
         <f>H28/(1-H$39)</f>
-        <v>0.72625698324022347</v>
-      </c>
-      <c r="I37" s="7">
-        <f t="shared" ref="I37:J37" si="12">I28/(1-I$39)</f>
-        <v>0</v>
-      </c>
+        <v>0.8106543138390272</v>
+      </c>
+      <c r="I37" s="7"/>
       <c r="J37" s="7">
-        <f t="shared" si="12"/>
-        <v>0.2</v>
-      </c>
-      <c r="K37" s="1"/>
-    </row>
-    <row r="38" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B38" s="4" t="s">
+        <f t="shared" ref="I37:J37" si="10">J28/(1-J$39)</f>
+        <v>0.31055900621118016</v>
+      </c>
+      <c r="K37" s="7">
+        <f t="shared" ref="K37" si="11">K28/(1-K$39)</f>
+        <v>0.15606710885680844</v>
+      </c>
+      <c r="L37" s="1"/>
+    </row>
+    <row r="38" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B38" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="C38" s="7">
+      <c r="C38" s="23">
         <f>C29/(1-C$39)</f>
-        <v>0.5494505494505495</v>
-      </c>
-      <c r="D38" s="7">
-        <f t="shared" si="11"/>
-        <v>0.55309734513274333</v>
-      </c>
-      <c r="E38" s="7">
-        <f t="shared" si="11"/>
-        <v>0.5298013245033113</v>
-      </c>
-      <c r="F38" s="7">
+        <v>0.38510734867344271</v>
+      </c>
+      <c r="D38" s="23">
+        <f>D29/(1-D$39)</f>
+        <v>0.43061023622047245</v>
+      </c>
+      <c r="E38" s="23">
+        <f>E29/(1-E$39)</f>
+        <v>0.40136176312488797</v>
+      </c>
+      <c r="F38" s="23">
         <f>F29/(1-F$39)</f>
-        <v>0.5</v>
-      </c>
-      <c r="G38" s="7">
+        <v>0.35</v>
+      </c>
+      <c r="G38" s="23">
         <f>G29/(1-G$39)</f>
-        <v>0.5</v>
-      </c>
-      <c r="H38" s="7">
+        <v>0.35</v>
+      </c>
+      <c r="H38" s="23">
         <f>H29/(1-H$39)</f>
-        <v>0.55865921787709494</v>
-      </c>
-      <c r="I38" s="7">
+        <v>0.4053271569195136</v>
+      </c>
+      <c r="I38" s="23">
         <f>I29/(1-I$39)</f>
-        <v>0.5181347150259068</v>
-      </c>
-      <c r="J38" s="7">
+        <v>0.36668412781561022</v>
+      </c>
+      <c r="J38" s="23">
         <f>J29/(1-J$39)</f>
-        <v>0.5</v>
-      </c>
-      <c r="K38" s="10"/>
-    </row>
-    <row r="39" spans="2:12" x14ac:dyDescent="0.25">
+        <v>0.43478260869565216</v>
+      </c>
+      <c r="K38" s="23">
+        <f>K29/(1-K$39)</f>
+        <v>0.43698790479906358</v>
+      </c>
+      <c r="L38" s="10"/>
+    </row>
+    <row r="39" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B39" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C39" s="11">
         <f>(1-C24)*(1-C25)*(1-C26)*(1-C27)*(1-C28)*(1-C29)</f>
-        <v>9.0000000000000024E-2</v>
+        <v>9.116249999999998E-2</v>
       </c>
       <c r="D39" s="11">
-        <f t="shared" ref="D39:I39" si="13">(1-D24)*(1-D25)*(1-D26)*(1-D27)*(1-D28)*(1-D29)</f>
-        <v>9.6000000000000002E-2</v>
+        <f t="shared" ref="D39:I39" si="12">(1-D24)*(1-D25)*(1-D26)*(1-D27)*(1-D28)*(1-D29)</f>
+        <v>0.18720000000000003</v>
       </c>
       <c r="E39" s="11">
-        <f t="shared" si="13"/>
-        <v>5.6250000000000008E-2</v>
+        <f t="shared" si="12"/>
+        <v>0.12796875000000002</v>
       </c>
       <c r="F39" s="11">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="G39" s="11">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="H39" s="11">
-        <f t="shared" si="13"/>
-        <v>0.105</v>
+        <f t="shared" si="12"/>
+        <v>0.13650000000000001</v>
       </c>
       <c r="I39" s="11">
-        <f t="shared" si="13"/>
-        <v>3.4999999999999989E-2</v>
+        <f t="shared" si="12"/>
+        <v>4.5499999999999985E-2</v>
       </c>
       <c r="J39" s="11">
         <f>(1-J24)*(1-J25)*(1-J26)*(1-J27)*(1-J28)*(1-J29)</f>
-        <v>0</v>
-      </c>
-      <c r="K39" s="1"/>
-      <c r="L39" t="s">
+        <v>0.19500000000000003</v>
+      </c>
+      <c r="K39" s="11">
+        <f>(1-K24)*(1-K25)*(1-K26)*(1-K27)*(1-K28)*(1-K29)</f>
+        <v>0.19906250000000003</v>
+      </c>
+      <c r="L39" s="1"/>
+      <c r="M39" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="40" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B40" s="13" t="s">
+    <row r="40" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B40" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="C40" s="14">
+      <c r="C40" s="25">
         <f>SUM(C33:C38)</f>
-        <v>1.8131868131868134</v>
-      </c>
-      <c r="D40" s="14">
-        <f t="shared" ref="D40:J40" si="14">SUM(D33:D38)</f>
-        <v>1.9911504424778763</v>
-      </c>
-      <c r="E40" s="14">
-        <f t="shared" si="14"/>
-        <v>2.0662251655629138</v>
-      </c>
-      <c r="F40" s="14">
-        <f t="shared" si="14"/>
-        <v>1.5</v>
-      </c>
-      <c r="G40" s="14">
-        <f t="shared" si="14"/>
-        <v>1.5</v>
-      </c>
-      <c r="H40" s="14">
-        <f t="shared" si="14"/>
-        <v>1.7318435754189943</v>
-      </c>
-      <c r="I40" s="14">
-        <f t="shared" si="14"/>
-        <v>1.7616580310880829</v>
-      </c>
-      <c r="J40" s="14">
-        <f t="shared" si="14"/>
-        <v>1.7</v>
-      </c>
-      <c r="L40" t="s">
+        <v>1.6229523979809373</v>
+      </c>
+      <c r="D40" s="25">
+        <f t="shared" ref="D40:J40" si="13">SUM(D33:D38)</f>
+        <v>1.5378937007874016</v>
+      </c>
+      <c r="E40" s="25">
+        <f t="shared" si="13"/>
+        <v>1.6341157498656154</v>
+      </c>
+      <c r="F40" s="25">
+        <f t="shared" si="13"/>
+        <v>1.35</v>
+      </c>
+      <c r="G40" s="25">
+        <f t="shared" si="13"/>
+        <v>1.35</v>
+      </c>
+      <c r="H40" s="25">
+        <f t="shared" si="13"/>
+        <v>1.5634047481181239</v>
+      </c>
+      <c r="I40" s="25">
+        <f t="shared" si="13"/>
+        <v>1.6238868517548455</v>
+      </c>
+      <c r="J40" s="25">
+        <f t="shared" si="13"/>
+        <v>1.4906832298136645</v>
+      </c>
+      <c r="K40" s="25">
+        <f t="shared" ref="K40" si="14">SUM(K33:K38)</f>
+        <v>1.498244245025361</v>
+      </c>
+      <c r="M40" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="41" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
@@ -1774,12 +1892,14 @@
       <c r="H41" s="2"/>
       <c r="I41" s="2"/>
       <c r="J41" s="2"/>
-    </row>
-    <row r="42" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="L42" s="2"/>
+      <c r="K41" s="2"/>
+    </row>
+    <row r="42" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="M42" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1787,7 +1907,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="C51" sqref="C51:F51"/>
     </sheetView>
   </sheetViews>
@@ -1800,7 +1920,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="18" t="s">
         <v>86</v>
       </c>
     </row>
@@ -1813,10 +1933,10 @@
       <c r="B4" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="20" t="s">
+      <c r="D4" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="F4" s="20" t="s">
+      <c r="F4" s="18" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1875,7 +1995,7 @@
       <c r="F8" t="s">
         <v>38</v>
       </c>
-      <c r="G8" s="20" t="s">
+      <c r="G8" s="18" t="s">
         <v>36</v>
       </c>
     </row>
@@ -2218,18 +2338,18 @@
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="20" t="s">
+      <c r="A43" s="18" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="20"/>
+      <c r="A44" s="18"/>
       <c r="B44" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C45" s="21" t="s">
+      <c r="C45" s="19" t="s">
         <v>87</v>
       </c>
       <c r="D45" t="s">
@@ -2238,19 +2358,19 @@
       <c r="E45" t="s">
         <v>28</v>
       </c>
-      <c r="F45" s="21" t="s">
+      <c r="F45" s="19" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C46" s="21"/>
+      <c r="C46" s="19"/>
       <c r="D46" t="s">
         <v>80</v>
       </c>
       <c r="E46" t="s">
         <v>28</v>
       </c>
-      <c r="F46" s="21"/>
+      <c r="F46" s="19"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C47" t="s">

</xml_diff>

<commit_message>
Corrige une erreur de calcul
En effet désormais certaines ressources sont distribuées en même temps
</commit_message>
<xml_diff>
--- a/Schémas.xlsx
+++ b/Schémas.xlsx
@@ -316,7 +316,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -352,8 +352,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -369,6 +376,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -410,7 +423,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -456,9 +469,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -477,6 +487,49 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -791,8 +844,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:U42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -811,16 +864,16 @@
       <c r="C3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="26" t="s">
+      <c r="D3" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="26" t="s">
+      <c r="E3" s="25" t="s">
         <v>7</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="26" t="s">
+      <c r="G3" s="25" t="s">
         <v>9</v>
       </c>
       <c r="H3" s="5" t="s">
@@ -847,7 +900,7 @@
       <c r="C4" s="6">
         <v>0.8</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="30">
         <v>0.1</v>
       </c>
       <c r="E4" s="6"/>
@@ -866,26 +919,26 @@
       </c>
     </row>
     <row r="5" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="21">
+      <c r="C5" s="20">
         <v>0.15</v>
       </c>
-      <c r="D5" s="21">
+      <c r="D5" s="31">
         <v>0.2</v>
       </c>
-      <c r="E5" s="21">
+      <c r="E5" s="20">
         <v>0.25</v>
       </c>
-      <c r="F5" s="21"/>
-      <c r="G5" s="21"/>
-      <c r="H5" s="21"/>
-      <c r="I5" s="21">
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="20">
         <v>0.9</v>
       </c>
-      <c r="J5" s="22"/>
-      <c r="K5" s="21">
+      <c r="J5" s="21"/>
+      <c r="K5" s="20">
         <v>0.125</v>
       </c>
     </row>
@@ -896,7 +949,7 @@
       <c r="C6" s="6">
         <v>0.17499999999999999</v>
       </c>
-      <c r="D6" s="6"/>
+      <c r="D6" s="30"/>
       <c r="E6" s="6"/>
       <c r="F6" s="6">
         <v>1</v>
@@ -912,30 +965,30 @@
       </c>
     </row>
     <row r="7" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B7" s="20" t="s">
+      <c r="B7" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21">
+      <c r="C7" s="20"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="20">
         <v>0.7</v>
       </c>
-      <c r="F7" s="21"/>
-      <c r="G7" s="21"/>
-      <c r="H7" s="21">
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="20">
         <v>0.3</v>
       </c>
-      <c r="I7" s="22"/>
-      <c r="J7" s="22"/>
-      <c r="K7" s="21"/>
-      <c r="M7" s="27"/>
+      <c r="I7" s="21"/>
+      <c r="J7" s="21"/>
+      <c r="K7" s="20"/>
+      <c r="M7" s="26"/>
     </row>
     <row r="8" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C8" s="6"/>
-      <c r="D8" s="6">
+      <c r="D8" s="30">
         <v>0.6</v>
       </c>
       <c r="E8" s="6">
@@ -955,20 +1008,20 @@
       </c>
     </row>
     <row r="9" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B9" s="20" t="s">
+      <c r="B9" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21">
+      <c r="C9" s="20"/>
+      <c r="D9" s="31">
         <v>0.35</v>
       </c>
-      <c r="E9" s="22"/>
-      <c r="F9" s="22"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="22"/>
-      <c r="I9" s="22"/>
-      <c r="J9" s="22"/>
-      <c r="K9" s="21"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="21"/>
+      <c r="I9" s="21"/>
+      <c r="J9" s="21"/>
+      <c r="K9" s="20"/>
       <c r="M9" s="8"/>
       <c r="N9" s="8"/>
       <c r="O9" s="8"/>
@@ -982,7 +1035,7 @@
     <row r="10" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B10" s="8"/>
       <c r="C10" s="14"/>
-      <c r="D10" s="13"/>
+      <c r="D10" s="32"/>
       <c r="E10" s="13"/>
       <c r="F10" s="13"/>
       <c r="G10" s="13"/>
@@ -1004,6 +1057,7 @@
       <c r="B11" t="s">
         <v>19</v>
       </c>
+      <c r="D11" s="33"/>
       <c r="M11" s="8"/>
       <c r="N11" s="8"/>
       <c r="O11" s="8"/>
@@ -1019,10 +1073,10 @@
       <c r="C12" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="26" t="s">
+      <c r="D12" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="26" t="s">
+      <c r="E12" s="25" t="s">
         <v>7</v>
       </c>
       <c r="F12" s="5" t="s">
@@ -1059,21 +1113,21 @@
       </c>
       <c r="C13" s="7">
         <f>C4/(1-C$19)</f>
-        <v>0.93050305321314342</v>
-      </c>
-      <c r="D13" s="7">
+        <v>0.92485549132947986</v>
+      </c>
+      <c r="D13" s="34">
         <f>D4/(1-D$19)</f>
-        <v>0.12303149606299214</v>
+        <v>0.12224938875305623</v>
       </c>
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
       <c r="G13" s="7">
-        <f t="shared" ref="D13:I13" si="0">G4/(1-G$19)</f>
+        <f>G4/(1-G$19)</f>
         <v>1</v>
       </c>
       <c r="H13" s="7"/>
       <c r="I13" s="7">
-        <f t="shared" si="0"/>
+        <f>I4/(1-I$19)</f>
         <v>0.32258064516129031</v>
       </c>
       <c r="J13" s="7"/>
@@ -1089,32 +1143,32 @@
       <c r="U13" s="8"/>
     </row>
     <row r="14" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B14" s="20" t="s">
+      <c r="B14" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C14" s="23">
+      <c r="C14" s="22">
         <f>C5/(1-C$19)</f>
-        <v>0.17446932247746438</v>
-      </c>
-      <c r="D14" s="23">
+        <v>0.17341040462427745</v>
+      </c>
+      <c r="D14" s="35">
         <f>D5/(1-D$19)</f>
-        <v>0.24606299212598429</v>
-      </c>
-      <c r="E14" s="23">
+        <v>0.24449877750611246</v>
+      </c>
+      <c r="E14" s="22">
         <f>E5/(1-E$19)</f>
-        <v>0.31128404669260701</v>
-      </c>
-      <c r="F14" s="23"/>
-      <c r="G14" s="23"/>
-      <c r="H14" s="23"/>
-      <c r="I14" s="23">
-        <f t="shared" ref="I14" si="1">I5/(1-I$19)</f>
+        <v>0.30769230769230771</v>
+      </c>
+      <c r="F14" s="22"/>
+      <c r="G14" s="22"/>
+      <c r="H14" s="22"/>
+      <c r="I14" s="22">
+        <f>I5/(1-I$19)</f>
         <v>0.96774193548387089</v>
       </c>
-      <c r="J14" s="23"/>
-      <c r="K14" s="23">
-        <f t="shared" ref="J14:K15" si="2">K5/(1-K$19)</f>
-        <v>0.1801801801801802</v>
+      <c r="J14" s="22"/>
+      <c r="K14" s="22">
+        <f>K5/(1-K$19)</f>
+        <v>0.17857142857142858</v>
       </c>
       <c r="M14" s="8"/>
       <c r="N14" s="8"/>
@@ -1132,9 +1186,9 @@
       </c>
       <c r="C15" s="7">
         <f>C6/(1-C$19)</f>
-        <v>0.2035475428903751</v>
-      </c>
-      <c r="D15" s="7"/>
+        <v>0.20231213872832368</v>
+      </c>
+      <c r="D15" s="34"/>
       <c r="E15" s="7"/>
       <c r="F15" s="7">
         <f>F6/(1-F$19)</f>
@@ -1144,12 +1198,12 @@
       <c r="H15" s="7"/>
       <c r="I15" s="7"/>
       <c r="J15" s="7">
-        <f t="shared" si="2"/>
+        <f>J6/(1-J$19)</f>
         <v>0.85714285714285721</v>
       </c>
       <c r="K15" s="7">
         <f>K6/(1-K$19)</f>
-        <v>0.86486486486486491</v>
+        <v>0.85714285714285721</v>
       </c>
       <c r="M15" s="13"/>
       <c r="N15" s="13"/>
@@ -1162,24 +1216,24 @@
       <c r="U15" s="8"/>
     </row>
     <row r="16" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B16" s="20" t="s">
+      <c r="B16" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="C16" s="23"/>
-      <c r="D16" s="23"/>
-      <c r="E16" s="23">
+      <c r="C16" s="22"/>
+      <c r="D16" s="35"/>
+      <c r="E16" s="22">
         <f>E7/(1-E$19)</f>
-        <v>0.87159533073929962</v>
-      </c>
-      <c r="F16" s="23"/>
-      <c r="G16" s="23"/>
-      <c r="H16" s="23">
+        <v>0.86153846153846148</v>
+      </c>
+      <c r="F16" s="22"/>
+      <c r="G16" s="22"/>
+      <c r="H16" s="22">
         <f>H7/(1-H$19)</f>
         <v>0.37974683544303794</v>
       </c>
-      <c r="I16" s="23"/>
-      <c r="J16" s="23"/>
-      <c r="K16" s="23"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
+      <c r="K16" s="22"/>
       <c r="M16" s="8"/>
       <c r="N16" s="8"/>
       <c r="O16" s="8"/>
@@ -1195,13 +1249,13 @@
         <v>4</v>
       </c>
       <c r="C17" s="7"/>
-      <c r="D17" s="7">
+      <c r="D17" s="34">
         <f>D8/(1-D$19)</f>
-        <v>0.73818897637795278</v>
+        <v>0.73349633251833735</v>
       </c>
       <c r="E17" s="7">
         <f>E8/(1-E$19)</f>
-        <v>0.1556420233463035</v>
+        <v>0.15384615384615385</v>
       </c>
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
@@ -1211,12 +1265,12 @@
       </c>
       <c r="I17" s="7"/>
       <c r="J17" s="7">
-        <f t="shared" ref="J17:K17" si="3">J8/(1-J$19)</f>
+        <f>J8/(1-J$19)</f>
         <v>0.35714285714285715</v>
       </c>
       <c r="K17" s="7">
-        <f t="shared" si="3"/>
-        <v>0.1801801801801802</v>
+        <f>K8/(1-K$19)</f>
+        <v>0.17857142857142858</v>
       </c>
       <c r="M17" s="8"/>
       <c r="N17" s="8"/>
@@ -1229,21 +1283,21 @@
       <c r="U17" s="8"/>
     </row>
     <row r="18" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B18" s="20" t="s">
+      <c r="B18" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="C18" s="23"/>
-      <c r="D18" s="23">
+      <c r="C18" s="22"/>
+      <c r="D18" s="35">
         <f>D9/(1-D$19)</f>
-        <v>0.43061023622047245</v>
-      </c>
-      <c r="E18" s="23"/>
-      <c r="F18" s="23"/>
-      <c r="G18" s="23"/>
-      <c r="H18" s="23"/>
-      <c r="I18" s="23"/>
-      <c r="J18" s="23"/>
-      <c r="K18" s="23"/>
+        <v>0.42787286063569674</v>
+      </c>
+      <c r="E18" s="22"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="22"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="22"/>
+      <c r="K18" s="22"/>
       <c r="M18" s="8"/>
       <c r="N18" s="8"/>
       <c r="O18" s="8"/>
@@ -1259,84 +1313,84 @@
         <v>13</v>
       </c>
       <c r="C19" s="11">
-        <f>(1-C4)*(1-C5)*(1-C6)*(1-C7)*(1-C8)*(1-C9)</f>
-        <v>0.14024999999999996</v>
-      </c>
-      <c r="D19" s="11">
-        <f>(1-D4)*(1-D5)*(1-D6)*(1-D7)*(1-D8)*(1-D9)</f>
-        <v>0.18720000000000003</v>
+        <f>(1-C4)*(1-C5-C6)</f>
+        <v>0.13499999999999998</v>
+      </c>
+      <c r="D19" s="36">
+        <f>(1-D4-D5)*(1-D8)*(1-D9)</f>
+        <v>0.182</v>
       </c>
       <c r="E19" s="11">
-        <f t="shared" ref="D19:K19" si="4">(1-E4)*(1-E5)*(1-E6)*(1-E7)*(1-E8)*(1-E9)</f>
-        <v>0.19687500000000002</v>
+        <f>(1-E7)*(1-E5-E8)</f>
+        <v>0.18750000000000003</v>
       </c>
       <c r="F19" s="11">
-        <f t="shared" si="4"/>
+        <f>(1-F6)</f>
         <v>0</v>
       </c>
       <c r="G19" s="11">
-        <f t="shared" si="4"/>
+        <f>(1-G4)</f>
         <v>0</v>
       </c>
       <c r="H19" s="11">
-        <f t="shared" si="4"/>
+        <f>(1-H4)*(1-H5)*(1-H6)*(1-H7)*(1-H8)*(1-H9)</f>
         <v>0.21000000000000002</v>
       </c>
       <c r="I19" s="11">
-        <f t="shared" si="4"/>
+        <f>(1-I4)*(1-I5)*(1-I6)*(1-I7)*(1-I8)*(1-I9)</f>
         <v>6.9999999999999979E-2</v>
       </c>
       <c r="J19" s="11">
-        <f t="shared" si="4"/>
+        <f>(1-J4)*(1-J5)*(1-J6)*(1-J7)*(1-J8)*(1-J9)</f>
         <v>0.30000000000000004</v>
       </c>
       <c r="K19" s="11">
-        <f t="shared" si="4"/>
-        <v>0.30625000000000002</v>
+        <f>(1-K6)*(1-K5-K8)</f>
+        <v>0.30000000000000004</v>
       </c>
       <c r="M19" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="20" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B20" s="24" t="s">
+      <c r="B20" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="C20" s="25">
+      <c r="C20" s="24">
         <f>SUM(C13:C18)</f>
-        <v>1.3085199185809828</v>
-      </c>
-      <c r="D20" s="25">
-        <f t="shared" ref="D20:I20" si="5">SUM(D13:D18)</f>
-        <v>1.5378937007874016</v>
-      </c>
-      <c r="E20" s="25">
-        <f t="shared" si="5"/>
-        <v>1.3385214007782102</v>
-      </c>
-      <c r="F20" s="25">
-        <f t="shared" si="5"/>
+        <v>1.300578034682081</v>
+      </c>
+      <c r="D20" s="37">
+        <f t="shared" ref="D20:I20" si="0">SUM(D13:D18)</f>
+        <v>1.5281173594132027</v>
+      </c>
+      <c r="E20" s="24">
+        <f t="shared" si="0"/>
+        <v>1.3230769230769228</v>
+      </c>
+      <c r="F20" s="24">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G20" s="25">
-        <f t="shared" si="5"/>
+      <c r="G20" s="24">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H20" s="25">
-        <f t="shared" si="5"/>
+      <c r="H20" s="24">
+        <f t="shared" si="0"/>
         <v>1.2658227848101264</v>
       </c>
-      <c r="I20" s="25">
-        <f t="shared" si="5"/>
+      <c r="I20" s="24">
+        <f t="shared" si="0"/>
         <v>1.2903225806451613</v>
       </c>
-      <c r="J20" s="25">
+      <c r="J20" s="24">
         <f>SUM(J13:J18)</f>
         <v>1.2142857142857144</v>
       </c>
-      <c r="K20" s="25">
+      <c r="K20" s="24">
         <f>SUM(K13:K18)</f>
-        <v>1.2252252252252251</v>
+        <v>1.2142857142857144</v>
       </c>
       <c r="M20" t="s">
         <v>21</v>
@@ -1345,7 +1399,7 @@
     <row r="21" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B21" s="15"/>
       <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
+      <c r="D21" s="38"/>
       <c r="E21" s="12"/>
       <c r="F21" s="12"/>
       <c r="G21" s="12"/>
@@ -1359,7 +1413,7 @@
         <v>17</v>
       </c>
       <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
+      <c r="D22" s="39"/>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
@@ -1373,7 +1427,7 @@
       <c r="C23" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="D23" s="25" t="s">
         <v>6</v>
       </c>
       <c r="E23" s="5" t="s">
@@ -1402,168 +1456,108 @@
       <c r="B24" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C24" s="6">
-        <f>C4</f>
-        <v>0.8</v>
-      </c>
-      <c r="D24" s="6">
-        <f>D4</f>
-        <v>0.1</v>
-      </c>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6">
-        <f>G4</f>
+      <c r="C24" s="40"/>
+      <c r="D24" s="41"/>
+      <c r="E24" s="40"/>
+      <c r="F24" s="40"/>
+      <c r="G24" s="40"/>
+      <c r="H24" s="40"/>
+      <c r="I24" s="40"/>
+      <c r="J24" s="40"/>
+      <c r="K24" s="40"/>
+    </row>
+    <row r="25" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B25" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="H24" s="6"/>
-      <c r="I24" s="6">
-        <f>I4</f>
-        <v>0.3</v>
-      </c>
-      <c r="J24" s="6"/>
-      <c r="K24" s="6"/>
-    </row>
-    <row r="25" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B25" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="C25" s="21">
-        <f>C5</f>
-        <v>0.15</v>
-      </c>
-      <c r="D25" s="21">
-        <f>D5</f>
-        <v>0.2</v>
-      </c>
-      <c r="E25" s="21">
-        <f>E5</f>
-        <v>0.25</v>
-      </c>
-      <c r="F25" s="21"/>
-      <c r="G25" s="21"/>
-      <c r="H25" s="21"/>
-      <c r="I25" s="21">
-        <f>I5</f>
-        <v>0.9</v>
-      </c>
-      <c r="J25" s="21"/>
-      <c r="K25" s="21">
-        <f>K5</f>
-        <v>0.125</v>
-      </c>
+      <c r="C25" s="40"/>
+      <c r="D25" s="41"/>
+      <c r="E25" s="40"/>
+      <c r="F25" s="40"/>
+      <c r="G25" s="40"/>
+      <c r="H25" s="40"/>
+      <c r="I25" s="40"/>
+      <c r="J25" s="40"/>
+      <c r="K25" s="40"/>
     </row>
     <row r="26" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B26" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C26" s="6">
-        <f>C6</f>
-        <v>0.17499999999999999</v>
-      </c>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="6">
-        <f>F6</f>
-        <v>1</v>
-      </c>
-      <c r="G26" s="6"/>
-      <c r="H26" s="6"/>
-      <c r="I26" s="6"/>
-      <c r="J26" s="6">
-        <f>J6</f>
-        <v>0.6</v>
-      </c>
-      <c r="K26" s="6">
-        <f>K6</f>
-        <v>0.6</v>
-      </c>
+      <c r="C26" s="40"/>
+      <c r="D26" s="41"/>
+      <c r="E26" s="40"/>
+      <c r="F26" s="40"/>
+      <c r="G26" s="40"/>
+      <c r="H26" s="40"/>
+      <c r="I26" s="40"/>
+      <c r="J26" s="40"/>
+      <c r="K26" s="40"/>
     </row>
     <row r="27" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B27" s="20" t="s">
+      <c r="B27" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="C27" s="21"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="21">
-        <f>E7</f>
-        <v>0.7</v>
-      </c>
-      <c r="F27" s="21"/>
-      <c r="G27" s="21"/>
-      <c r="H27" s="21">
-        <f>H7</f>
-        <v>0.3</v>
-      </c>
-      <c r="I27" s="21"/>
-      <c r="J27" s="21"/>
-      <c r="K27" s="21"/>
+      <c r="C27" s="40"/>
+      <c r="D27" s="41"/>
+      <c r="E27" s="40"/>
+      <c r="F27" s="40"/>
+      <c r="G27" s="40"/>
+      <c r="H27" s="40"/>
+      <c r="I27" s="40"/>
+      <c r="J27" s="40"/>
+      <c r="K27" s="40"/>
     </row>
     <row r="28" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B28" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6">
-        <f>D8</f>
-        <v>0.6</v>
-      </c>
-      <c r="E28" s="6">
-        <f>E8</f>
-        <v>0.125</v>
-      </c>
-      <c r="F28" s="6"/>
-      <c r="G28" s="6"/>
-      <c r="H28" s="6">
-        <f>H8</f>
-        <v>0.7</v>
-      </c>
-      <c r="I28" s="6"/>
-      <c r="J28" s="6">
-        <f>J8</f>
-        <v>0.25</v>
-      </c>
-      <c r="K28" s="6">
-        <f>K8</f>
-        <v>0.125</v>
-      </c>
+      <c r="C28" s="40"/>
+      <c r="D28" s="41"/>
+      <c r="E28" s="40"/>
+      <c r="F28" s="40"/>
+      <c r="G28" s="40"/>
+      <c r="H28" s="40"/>
+      <c r="I28" s="40"/>
+      <c r="J28" s="40"/>
+      <c r="K28" s="40"/>
     </row>
     <row r="29" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B29" s="20" t="s">
+      <c r="B29" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="C29" s="21">
+      <c r="C29" s="20">
         <v>0.35</v>
       </c>
-      <c r="D29" s="21">
+      <c r="D29" s="31">
+        <v>0</v>
+      </c>
+      <c r="E29" s="20">
         <v>0.35</v>
       </c>
-      <c r="E29" s="21">
+      <c r="F29" s="20">
         <v>0.35</v>
       </c>
-      <c r="F29" s="21">
+      <c r="G29" s="20">
         <v>0.35</v>
       </c>
-      <c r="G29" s="21">
+      <c r="H29" s="20">
         <v>0.35</v>
       </c>
-      <c r="H29" s="21">
+      <c r="I29" s="20">
         <v>0.35</v>
       </c>
-      <c r="I29" s="21">
+      <c r="J29" s="20">
         <v>0.35</v>
       </c>
-      <c r="J29" s="21">
-        <v>0.35</v>
-      </c>
-      <c r="K29" s="21">
+      <c r="K29" s="20">
         <v>0.35</v>
       </c>
     </row>
     <row r="30" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B30" s="8"/>
       <c r="C30" s="14"/>
-      <c r="D30" s="14"/>
+      <c r="D30" s="28"/>
       <c r="E30" s="14"/>
       <c r="F30" s="14"/>
       <c r="G30" s="14"/>
@@ -1577,7 +1571,7 @@
         <v>16</v>
       </c>
       <c r="C31" s="9"/>
-      <c r="D31" s="9"/>
+      <c r="D31" s="29"/>
       <c r="E31" s="9"/>
       <c r="F31" s="9"/>
       <c r="G31" s="9"/>
@@ -1591,7 +1585,7 @@
       <c r="C32" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D32" s="5" t="s">
+      <c r="D32" s="25" t="s">
         <v>6</v>
       </c>
       <c r="E32" s="5" t="s">
@@ -1622,22 +1616,22 @@
         <v>0</v>
       </c>
       <c r="C33" s="7">
-        <f>C24/(1-C$39)</f>
-        <v>0.88024536839644063</v>
-      </c>
-      <c r="D33" s="7">
-        <f t="shared" ref="D33:I33" si="6">D24/(1-D$39)</f>
-        <v>0.12303149606299214</v>
+        <f>C4/(1-C$39)</f>
+        <v>0.87695258975061663</v>
+      </c>
+      <c r="D33" s="34">
+        <f>D4/(1-D$39)</f>
+        <v>0.1388888888888889</v>
       </c>
       <c r="E33" s="7"/>
       <c r="F33" s="7"/>
       <c r="G33" s="7">
-        <f t="shared" si="6"/>
+        <f>G4/(1-G$39)</f>
         <v>1</v>
       </c>
       <c r="H33" s="7"/>
       <c r="I33" s="7">
-        <f t="shared" si="6"/>
+        <f>I4/(1-I$39)</f>
         <v>0.31430068098480879</v>
       </c>
       <c r="J33" s="7"/>
@@ -1645,32 +1639,32 @@
       <c r="L33" s="1"/>
     </row>
     <row r="34" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B34" s="20" t="s">
+      <c r="B34" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C34" s="23">
-        <f>C25/(1-C$39)</f>
-        <v>0.1650460065743326</v>
-      </c>
-      <c r="D34" s="23">
-        <f>D25/(1-D$39)</f>
-        <v>0.24606299212598429</v>
-      </c>
-      <c r="E34" s="23">
-        <f>E25/(1-E$39)</f>
-        <v>0.28668697366063428</v>
-      </c>
-      <c r="F34" s="23"/>
-      <c r="G34" s="23"/>
-      <c r="H34" s="23"/>
-      <c r="I34" s="23">
-        <f t="shared" ref="F34:J34" si="7">I25/(1-I$39)</f>
+      <c r="C34" s="22">
+        <f>C5/(1-C$39)</f>
+        <v>0.1644286105782406</v>
+      </c>
+      <c r="D34" s="35">
+        <f>D5/(1-D$39)</f>
+        <v>0.27777777777777779</v>
+      </c>
+      <c r="E34" s="22">
+        <f>E5/(1-E$39)</f>
+        <v>0.28469750889679718</v>
+      </c>
+      <c r="F34" s="22"/>
+      <c r="G34" s="22"/>
+      <c r="H34" s="22"/>
+      <c r="I34" s="22">
+        <f>I5/(1-I$39)</f>
         <v>0.94290204295442637</v>
       </c>
-      <c r="J34" s="23"/>
-      <c r="K34" s="23">
-        <f t="shared" ref="K34" si="8">K25/(1-K$39)</f>
-        <v>0.15606710885680844</v>
+      <c r="J34" s="22"/>
+      <c r="K34" s="22">
+        <f>K5/(1-K$39)</f>
+        <v>0.15527950310559008</v>
       </c>
       <c r="L34" s="1"/>
     </row>
@@ -1679,47 +1673,47 @@
         <v>2</v>
       </c>
       <c r="C35" s="7">
-        <f>C26/(1-C$39)</f>
-        <v>0.19255367433672135</v>
-      </c>
-      <c r="D35" s="7"/>
+        <f>C6/(1-C$39)</f>
+        <v>0.19183337900794736</v>
+      </c>
+      <c r="D35" s="34"/>
       <c r="E35" s="7"/>
       <c r="F35" s="7">
-        <f>F26/(1-F$39)</f>
+        <f>F6/(1-F$39)</f>
         <v>1</v>
       </c>
       <c r="G35" s="7"/>
       <c r="H35" s="7"/>
       <c r="I35" s="7"/>
       <c r="J35" s="7">
-        <f t="shared" ref="J35:K35" si="9">J26/(1-J$39)</f>
+        <f>J6/(1-J$39)</f>
         <v>0.74534161490683237</v>
       </c>
       <c r="K35" s="7">
-        <f t="shared" si="9"/>
-        <v>0.7491221225126804</v>
+        <f>K6/(1-K$39)</f>
+        <v>0.74534161490683237</v>
       </c>
       <c r="L35" s="1"/>
     </row>
     <row r="36" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B36" s="20" t="s">
+      <c r="B36" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="C36" s="23"/>
-      <c r="D36" s="23"/>
-      <c r="E36" s="23">
-        <f>E27/(1-E$39)</f>
-        <v>0.80272352624977594</v>
-      </c>
-      <c r="F36" s="23"/>
-      <c r="G36" s="23"/>
-      <c r="H36" s="23">
-        <f>H27/(1-H$39)</f>
+      <c r="C36" s="22"/>
+      <c r="D36" s="35"/>
+      <c r="E36" s="22">
+        <f>E7/(1-E$39)</f>
+        <v>0.79715302491103202</v>
+      </c>
+      <c r="F36" s="22"/>
+      <c r="G36" s="22"/>
+      <c r="H36" s="22">
+        <f>H7/(1-H$39)</f>
         <v>0.34742327735958312</v>
       </c>
-      <c r="I36" s="23"/>
-      <c r="J36" s="23"/>
-      <c r="K36" s="23"/>
+      <c r="I36" s="22"/>
+      <c r="J36" s="22"/>
+      <c r="K36" s="22"/>
       <c r="L36" s="1"/>
     </row>
     <row r="37" spans="2:13" x14ac:dyDescent="0.25">
@@ -1727,70 +1721,67 @@
         <v>4</v>
       </c>
       <c r="C37" s="7"/>
-      <c r="D37" s="7">
-        <f>D28/(1-D$39)</f>
-        <v>0.73818897637795278</v>
+      <c r="D37" s="34">
+        <f>D8/(1-D$39)</f>
+        <v>0.83333333333333337</v>
       </c>
       <c r="E37" s="7">
-        <f>E28/(1-E$39)</f>
-        <v>0.14334348683031714</v>
+        <f>E8/(1-E$39)</f>
+        <v>0.14234875444839859</v>
       </c>
       <c r="F37" s="7"/>
       <c r="G37" s="7"/>
       <c r="H37" s="7">
-        <f>H28/(1-H$39)</f>
+        <f>H8/(1-H$39)</f>
         <v>0.8106543138390272</v>
       </c>
       <c r="I37" s="7"/>
       <c r="J37" s="7">
-        <f t="shared" ref="I37:J37" si="10">J28/(1-J$39)</f>
+        <f>J8/(1-J$39)</f>
         <v>0.31055900621118016</v>
       </c>
       <c r="K37" s="7">
-        <f t="shared" ref="K37" si="11">K28/(1-K$39)</f>
-        <v>0.15606710885680844</v>
+        <f>K8/(1-K$39)</f>
+        <v>0.15527950310559008</v>
       </c>
       <c r="L37" s="1"/>
     </row>
     <row r="38" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B38" s="20" t="s">
+      <c r="B38" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="C38" s="23">
+      <c r="C38" s="22">
         <f>C29/(1-C$39)</f>
-        <v>0.38510734867344271</v>
-      </c>
-      <c r="D38" s="23">
-        <f>D29/(1-D$39)</f>
-        <v>0.43061023622047245</v>
-      </c>
-      <c r="E38" s="23">
+        <v>0.38366675801589473</v>
+      </c>
+      <c r="D38" s="35"/>
+      <c r="E38" s="22">
         <f>E29/(1-E$39)</f>
-        <v>0.40136176312488797</v>
-      </c>
-      <c r="F38" s="23">
+        <v>0.39857651245551601</v>
+      </c>
+      <c r="F38" s="22">
         <f>F29/(1-F$39)</f>
         <v>0.35</v>
       </c>
-      <c r="G38" s="23">
+      <c r="G38" s="22">
         <f>G29/(1-G$39)</f>
         <v>0.35</v>
       </c>
-      <c r="H38" s="23">
+      <c r="H38" s="22">
         <f>H29/(1-H$39)</f>
         <v>0.4053271569195136</v>
       </c>
-      <c r="I38" s="23">
+      <c r="I38" s="22">
         <f>I29/(1-I$39)</f>
         <v>0.36668412781561022</v>
       </c>
-      <c r="J38" s="23">
+      <c r="J38" s="22">
         <f>J29/(1-J$39)</f>
         <v>0.43478260869565216</v>
       </c>
-      <c r="K38" s="23">
+      <c r="K38" s="22">
         <f>K29/(1-K$39)</f>
-        <v>0.43698790479906358</v>
+        <v>0.43478260869565216</v>
       </c>
       <c r="L38" s="10"/>
     </row>
@@ -1799,40 +1790,40 @@
         <v>13</v>
       </c>
       <c r="C39" s="11">
-        <f>(1-C24)*(1-C25)*(1-C26)*(1-C27)*(1-C28)*(1-C29)</f>
-        <v>9.116249999999998E-2</v>
+        <f>C19*(1-C29)</f>
+        <v>8.7749999999999995E-2</v>
       </c>
       <c r="D39" s="11">
-        <f t="shared" ref="D39:I39" si="12">(1-D24)*(1-D25)*(1-D26)*(1-D27)*(1-D28)*(1-D29)</f>
-        <v>0.18720000000000003</v>
+        <f>(1-D4-D5)*(1-D8)</f>
+        <v>0.27999999999999997</v>
       </c>
       <c r="E39" s="11">
-        <f t="shared" si="12"/>
-        <v>0.12796875000000002</v>
+        <f>E19*(1-E29)</f>
+        <v>0.12187500000000002</v>
       </c>
       <c r="F39" s="11">
-        <f t="shared" si="12"/>
+        <f>F19*(1-F29)</f>
         <v>0</v>
       </c>
       <c r="G39" s="11">
-        <f t="shared" si="12"/>
+        <f>G19*(1-G29)</f>
         <v>0</v>
       </c>
       <c r="H39" s="11">
-        <f t="shared" si="12"/>
+        <f t="shared" ref="H39:K39" si="1">H19*(1-H29)</f>
         <v>0.13650000000000001</v>
       </c>
       <c r="I39" s="11">
-        <f t="shared" si="12"/>
+        <f t="shared" si="1"/>
         <v>4.5499999999999985E-2</v>
       </c>
       <c r="J39" s="11">
-        <f>(1-J24)*(1-J25)*(1-J26)*(1-J27)*(1-J28)*(1-J29)</f>
+        <f t="shared" si="1"/>
         <v>0.19500000000000003</v>
       </c>
       <c r="K39" s="11">
-        <f>(1-K24)*(1-K25)*(1-K26)*(1-K27)*(1-K28)*(1-K29)</f>
-        <v>0.19906250000000003</v>
+        <f t="shared" si="1"/>
+        <v>0.19500000000000003</v>
       </c>
       <c r="L39" s="1"/>
       <c r="M39" t="s">
@@ -1840,44 +1831,44 @@
       </c>
     </row>
     <row r="40" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B40" s="24" t="s">
+      <c r="B40" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="C40" s="25">
+      <c r="C40" s="24">
         <f>SUM(C33:C38)</f>
-        <v>1.6229523979809373</v>
-      </c>
-      <c r="D40" s="25">
-        <f t="shared" ref="D40:J40" si="13">SUM(D33:D38)</f>
-        <v>1.5378937007874016</v>
-      </c>
-      <c r="E40" s="25">
-        <f t="shared" si="13"/>
-        <v>1.6341157498656154</v>
-      </c>
-      <c r="F40" s="25">
-        <f t="shared" si="13"/>
+        <v>1.6168813373526993</v>
+      </c>
+      <c r="D40" s="37">
+        <f t="shared" ref="D40:J40" si="2">SUM(D33:D38)</f>
+        <v>1.25</v>
+      </c>
+      <c r="E40" s="24">
+        <f t="shared" si="2"/>
+        <v>1.6227758007117439</v>
+      </c>
+      <c r="F40" s="24">
+        <f t="shared" si="2"/>
         <v>1.35</v>
       </c>
-      <c r="G40" s="25">
-        <f t="shared" si="13"/>
+      <c r="G40" s="24">
+        <f t="shared" si="2"/>
         <v>1.35</v>
       </c>
-      <c r="H40" s="25">
-        <f t="shared" si="13"/>
+      <c r="H40" s="24">
+        <f t="shared" si="2"/>
         <v>1.5634047481181239</v>
       </c>
-      <c r="I40" s="25">
-        <f t="shared" si="13"/>
+      <c r="I40" s="24">
+        <f t="shared" si="2"/>
         <v>1.6238868517548455</v>
       </c>
-      <c r="J40" s="25">
-        <f t="shared" si="13"/>
+      <c r="J40" s="24">
+        <f t="shared" si="2"/>
         <v>1.4906832298136645</v>
       </c>
-      <c r="K40" s="25">
-        <f t="shared" ref="K40" si="14">SUM(K33:K38)</f>
-        <v>1.498244245025361</v>
+      <c r="K40" s="24">
+        <f t="shared" ref="K40" si="3">SUM(K33:K38)</f>
+        <v>1.4906832298136645</v>
       </c>
       <c r="M40" t="s">
         <v>21</v>
@@ -2349,7 +2340,7 @@
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C45" s="19" t="s">
+      <c r="C45" s="27" t="s">
         <v>87</v>
       </c>
       <c r="D45" t="s">
@@ -2358,19 +2349,19 @@
       <c r="E45" t="s">
         <v>28</v>
       </c>
-      <c r="F45" s="19" t="s">
+      <c r="F45" s="27" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C46" s="19"/>
+      <c r="C46" s="27"/>
       <c r="D46" t="s">
         <v>80</v>
       </c>
       <c r="E46" t="s">
         <v>28</v>
       </c>
-      <c r="F46" s="19"/>
+      <c r="F46" s="27"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C47" t="s">

</xml_diff>

<commit_message>
Mise à jour schéma + correction oubli + nettoyage
- Mise à jour du schéma avec l'augmentation de proba pour les ressources
doublées
- Correction de l'oubli de cette modification pour les plaines
- Retrait des commentaires signalant une modification puisque désormais
on a un gestionnaire de version qui fait cela mieux
</commit_message>
<xml_diff>
--- a/Schémas.xlsx
+++ b/Schémas.xlsx
@@ -487,9 +487,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -529,6 +526,9 @@
     </xf>
     <xf numFmtId="9" fontId="4" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -844,8 +844,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:U42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -900,8 +900,8 @@
       <c r="C4" s="6">
         <v>0.8</v>
       </c>
-      <c r="D4" s="30">
-        <v>0.1</v>
+      <c r="D4" s="29">
+        <v>0.2</v>
       </c>
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
@@ -923,13 +923,13 @@
         <v>1</v>
       </c>
       <c r="C5" s="20">
-        <v>0.15</v>
-      </c>
-      <c r="D5" s="31">
-        <v>0.2</v>
+        <v>0.3</v>
+      </c>
+      <c r="D5" s="30">
+        <v>0.4</v>
       </c>
       <c r="E5" s="20">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="F5" s="20"/>
       <c r="G5" s="20"/>
@@ -939,7 +939,7 @@
       </c>
       <c r="J5" s="21"/>
       <c r="K5" s="20">
-        <v>0.125</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="6" spans="2:21" x14ac:dyDescent="0.25">
@@ -947,9 +947,9 @@
         <v>2</v>
       </c>
       <c r="C6" s="6">
-        <v>0.17499999999999999</v>
-      </c>
-      <c r="D6" s="30"/>
+        <v>0.35</v>
+      </c>
+      <c r="D6" s="29"/>
       <c r="E6" s="6"/>
       <c r="F6" s="6">
         <v>1</v>
@@ -969,7 +969,7 @@
         <v>3</v>
       </c>
       <c r="C7" s="20"/>
-      <c r="D7" s="31"/>
+      <c r="D7" s="30"/>
       <c r="E7" s="20">
         <v>0.7</v>
       </c>
@@ -988,11 +988,11 @@
         <v>4</v>
       </c>
       <c r="C8" s="6"/>
-      <c r="D8" s="30">
+      <c r="D8" s="29">
         <v>0.6</v>
       </c>
       <c r="E8" s="6">
-        <v>0.125</v>
+        <v>0.25</v>
       </c>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
@@ -1004,7 +1004,7 @@
         <v>0.25</v>
       </c>
       <c r="K8" s="6">
-        <v>0.125</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="9" spans="2:21" x14ac:dyDescent="0.25">
@@ -1012,7 +1012,7 @@
         <v>12</v>
       </c>
       <c r="C9" s="20"/>
-      <c r="D9" s="31">
+      <c r="D9" s="30">
         <v>0.35</v>
       </c>
       <c r="E9" s="21"/>
@@ -1035,7 +1035,7 @@
     <row r="10" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B10" s="8"/>
       <c r="C10" s="14"/>
-      <c r="D10" s="32"/>
+      <c r="D10" s="31"/>
       <c r="E10" s="13"/>
       <c r="F10" s="13"/>
       <c r="G10" s="13"/>
@@ -1057,7 +1057,7 @@
       <c r="B11" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="33"/>
+      <c r="D11" s="32"/>
       <c r="M11" s="8"/>
       <c r="N11" s="8"/>
       <c r="O11" s="8"/>
@@ -1113,11 +1113,11 @@
       </c>
       <c r="C13" s="7">
         <f>C4/(1-C$19)</f>
-        <v>0.92485549132947986</v>
-      </c>
-      <c r="D13" s="34">
+        <v>0.86021505376344087</v>
+      </c>
+      <c r="D13" s="33">
         <f>D4/(1-D$19)</f>
-        <v>0.12224938875305623</v>
+        <v>0.22321428571428573</v>
       </c>
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
@@ -1148,15 +1148,15 @@
       </c>
       <c r="C14" s="22">
         <f>C5/(1-C$19)</f>
-        <v>0.17341040462427745</v>
-      </c>
-      <c r="D14" s="35">
+        <v>0.32258064516129031</v>
+      </c>
+      <c r="D14" s="34">
         <f>D5/(1-D$19)</f>
-        <v>0.24449877750611246</v>
+        <v>0.44642857142857145</v>
       </c>
       <c r="E14" s="22">
         <f>E5/(1-E$19)</f>
-        <v>0.30769230769230771</v>
+        <v>0.54054054054054046</v>
       </c>
       <c r="F14" s="22"/>
       <c r="G14" s="22"/>
@@ -1168,7 +1168,7 @@
       <c r="J14" s="22"/>
       <c r="K14" s="22">
         <f>K5/(1-K$19)</f>
-        <v>0.17857142857142858</v>
+        <v>0.3125</v>
       </c>
       <c r="M14" s="8"/>
       <c r="N14" s="8"/>
@@ -1186,9 +1186,9 @@
       </c>
       <c r="C15" s="7">
         <f>C6/(1-C$19)</f>
-        <v>0.20231213872832368</v>
-      </c>
-      <c r="D15" s="34"/>
+        <v>0.37634408602150532</v>
+      </c>
+      <c r="D15" s="33"/>
       <c r="E15" s="7"/>
       <c r="F15" s="7">
         <f>F6/(1-F$19)</f>
@@ -1203,7 +1203,7 @@
       </c>
       <c r="K15" s="7">
         <f>K6/(1-K$19)</f>
-        <v>0.85714285714285721</v>
+        <v>0.74999999999999989</v>
       </c>
       <c r="M15" s="13"/>
       <c r="N15" s="13"/>
@@ -1220,10 +1220,10 @@
         <v>3</v>
       </c>
       <c r="C16" s="22"/>
-      <c r="D16" s="35"/>
+      <c r="D16" s="34"/>
       <c r="E16" s="22">
         <f>E7/(1-E$19)</f>
-        <v>0.86153846153846148</v>
+        <v>0.75675675675675669</v>
       </c>
       <c r="F16" s="22"/>
       <c r="G16" s="22"/>
@@ -1249,13 +1249,13 @@
         <v>4</v>
       </c>
       <c r="C17" s="7"/>
-      <c r="D17" s="34">
+      <c r="D17" s="33">
         <f>D8/(1-D$19)</f>
-        <v>0.73349633251833735</v>
+        <v>0.6696428571428571</v>
       </c>
       <c r="E17" s="7">
         <f>E8/(1-E$19)</f>
-        <v>0.15384615384615385</v>
+        <v>0.27027027027027023</v>
       </c>
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
@@ -1270,7 +1270,7 @@
       </c>
       <c r="K17" s="7">
         <f>K8/(1-K$19)</f>
-        <v>0.17857142857142858</v>
+        <v>0.3125</v>
       </c>
       <c r="M17" s="8"/>
       <c r="N17" s="8"/>
@@ -1287,9 +1287,9 @@
         <v>12</v>
       </c>
       <c r="C18" s="22"/>
-      <c r="D18" s="35">
+      <c r="D18" s="34">
         <f>D9/(1-D$19)</f>
-        <v>0.42787286063569674</v>
+        <v>0.39062499999999994</v>
       </c>
       <c r="E18" s="22"/>
       <c r="F18" s="22"/>
@@ -1314,15 +1314,15 @@
       </c>
       <c r="C19" s="11">
         <f>(1-C4)*(1-C5-C6)</f>
-        <v>0.13499999999999998</v>
-      </c>
-      <c r="D19" s="36">
+        <v>6.9999999999999979E-2</v>
+      </c>
+      <c r="D19" s="35">
         <f>(1-D4-D5)*(1-D8)*(1-D9)</f>
-        <v>0.182</v>
+        <v>0.10400000000000002</v>
       </c>
       <c r="E19" s="11">
         <f>(1-E7)*(1-E5-E8)</f>
-        <v>0.18750000000000003</v>
+        <v>7.5000000000000011E-2</v>
       </c>
       <c r="F19" s="11">
         <f>(1-F6)</f>
@@ -1346,7 +1346,7 @@
       </c>
       <c r="K19" s="11">
         <f>(1-K6)*(1-K5-K8)</f>
-        <v>0.30000000000000004</v>
+        <v>0.2</v>
       </c>
       <c r="M19" t="s">
         <v>22</v>
@@ -1358,15 +1358,15 @@
       </c>
       <c r="C20" s="24">
         <f>SUM(C13:C18)</f>
-        <v>1.300578034682081</v>
-      </c>
-      <c r="D20" s="37">
+        <v>1.5591397849462365</v>
+      </c>
+      <c r="D20" s="36">
         <f t="shared" ref="D20:I20" si="0">SUM(D13:D18)</f>
-        <v>1.5281173594132027</v>
+        <v>1.7299107142857144</v>
       </c>
       <c r="E20" s="24">
         <f t="shared" si="0"/>
-        <v>1.3230769230769228</v>
+        <v>1.5675675675675673</v>
       </c>
       <c r="F20" s="24">
         <f t="shared" si="0"/>
@@ -1390,7 +1390,7 @@
       </c>
       <c r="K20" s="24">
         <f>SUM(K13:K18)</f>
-        <v>1.2142857142857144</v>
+        <v>1.375</v>
       </c>
       <c r="M20" t="s">
         <v>21</v>
@@ -1399,7 +1399,7 @@
     <row r="21" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B21" s="15"/>
       <c r="C21" s="12"/>
-      <c r="D21" s="38"/>
+      <c r="D21" s="37"/>
       <c r="E21" s="12"/>
       <c r="F21" s="12"/>
       <c r="G21" s="12"/>
@@ -1413,7 +1413,7 @@
         <v>17</v>
       </c>
       <c r="C22" s="3"/>
-      <c r="D22" s="39"/>
+      <c r="D22" s="38"/>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
@@ -1456,71 +1456,71 @@
       <c r="B24" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C24" s="40"/>
-      <c r="D24" s="41"/>
-      <c r="E24" s="40"/>
-      <c r="F24" s="40"/>
-      <c r="G24" s="40"/>
-      <c r="H24" s="40"/>
-      <c r="I24" s="40"/>
-      <c r="J24" s="40"/>
-      <c r="K24" s="40"/>
+      <c r="C24" s="39"/>
+      <c r="D24" s="40"/>
+      <c r="E24" s="39"/>
+      <c r="F24" s="39"/>
+      <c r="G24" s="39"/>
+      <c r="H24" s="39"/>
+      <c r="I24" s="39"/>
+      <c r="J24" s="39"/>
+      <c r="K24" s="39"/>
     </row>
     <row r="25" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B25" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C25" s="40"/>
-      <c r="D25" s="41"/>
-      <c r="E25" s="40"/>
-      <c r="F25" s="40"/>
-      <c r="G25" s="40"/>
-      <c r="H25" s="40"/>
-      <c r="I25" s="40"/>
-      <c r="J25" s="40"/>
-      <c r="K25" s="40"/>
+      <c r="C25" s="39"/>
+      <c r="D25" s="40"/>
+      <c r="E25" s="39"/>
+      <c r="F25" s="39"/>
+      <c r="G25" s="39"/>
+      <c r="H25" s="39"/>
+      <c r="I25" s="39"/>
+      <c r="J25" s="39"/>
+      <c r="K25" s="39"/>
     </row>
     <row r="26" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B26" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C26" s="40"/>
-      <c r="D26" s="41"/>
-      <c r="E26" s="40"/>
-      <c r="F26" s="40"/>
-      <c r="G26" s="40"/>
-      <c r="H26" s="40"/>
-      <c r="I26" s="40"/>
-      <c r="J26" s="40"/>
-      <c r="K26" s="40"/>
+      <c r="C26" s="39"/>
+      <c r="D26" s="40"/>
+      <c r="E26" s="39"/>
+      <c r="F26" s="39"/>
+      <c r="G26" s="39"/>
+      <c r="H26" s="39"/>
+      <c r="I26" s="39"/>
+      <c r="J26" s="39"/>
+      <c r="K26" s="39"/>
     </row>
     <row r="27" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B27" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="C27" s="40"/>
-      <c r="D27" s="41"/>
-      <c r="E27" s="40"/>
-      <c r="F27" s="40"/>
-      <c r="G27" s="40"/>
-      <c r="H27" s="40"/>
-      <c r="I27" s="40"/>
-      <c r="J27" s="40"/>
-      <c r="K27" s="40"/>
+      <c r="C27" s="39"/>
+      <c r="D27" s="40"/>
+      <c r="E27" s="39"/>
+      <c r="F27" s="39"/>
+      <c r="G27" s="39"/>
+      <c r="H27" s="39"/>
+      <c r="I27" s="39"/>
+      <c r="J27" s="39"/>
+      <c r="K27" s="39"/>
     </row>
     <row r="28" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B28" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C28" s="40"/>
-      <c r="D28" s="41"/>
-      <c r="E28" s="40"/>
-      <c r="F28" s="40"/>
-      <c r="G28" s="40"/>
-      <c r="H28" s="40"/>
-      <c r="I28" s="40"/>
-      <c r="J28" s="40"/>
-      <c r="K28" s="40"/>
+      <c r="C28" s="39"/>
+      <c r="D28" s="40"/>
+      <c r="E28" s="39"/>
+      <c r="F28" s="39"/>
+      <c r="G28" s="39"/>
+      <c r="H28" s="39"/>
+      <c r="I28" s="39"/>
+      <c r="J28" s="39"/>
+      <c r="K28" s="39"/>
     </row>
     <row r="29" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B29" s="19" t="s">
@@ -1529,8 +1529,8 @@
       <c r="C29" s="20">
         <v>0.35</v>
       </c>
-      <c r="D29" s="31">
-        <v>0</v>
+      <c r="D29" s="30">
+        <v>0.35</v>
       </c>
       <c r="E29" s="20">
         <v>0.35</v>
@@ -1557,7 +1557,7 @@
     <row r="30" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B30" s="8"/>
       <c r="C30" s="14"/>
-      <c r="D30" s="28"/>
+      <c r="D30" s="27"/>
       <c r="E30" s="14"/>
       <c r="F30" s="14"/>
       <c r="G30" s="14"/>
@@ -1571,7 +1571,7 @@
         <v>16</v>
       </c>
       <c r="C31" s="9"/>
-      <c r="D31" s="29"/>
+      <c r="D31" s="28"/>
       <c r="E31" s="9"/>
       <c r="F31" s="9"/>
       <c r="G31" s="9"/>
@@ -1617,11 +1617,11 @@
       </c>
       <c r="C33" s="7">
         <f>C4/(1-C$39)</f>
-        <v>0.87695258975061663</v>
-      </c>
-      <c r="D33" s="34">
+        <v>0.83813514929282351</v>
+      </c>
+      <c r="D33" s="33">
         <f>D4/(1-D$39)</f>
-        <v>0.1388888888888889</v>
+        <v>0.23809523809523811</v>
       </c>
       <c r="E33" s="7"/>
       <c r="F33" s="7"/>
@@ -1644,15 +1644,15 @@
       </c>
       <c r="C34" s="22">
         <f>C5/(1-C$39)</f>
-        <v>0.1644286105782406</v>
-      </c>
-      <c r="D34" s="35">
+        <v>0.31430068098480879</v>
+      </c>
+      <c r="D34" s="34">
         <f>D5/(1-D$39)</f>
-        <v>0.27777777777777779</v>
+        <v>0.47619047619047622</v>
       </c>
       <c r="E34" s="22">
         <f>E5/(1-E$39)</f>
-        <v>0.28469750889679718</v>
+        <v>0.52562417871222078</v>
       </c>
       <c r="F34" s="22"/>
       <c r="G34" s="22"/>
@@ -1664,7 +1664,7 @@
       <c r="J34" s="22"/>
       <c r="K34" s="22">
         <f>K5/(1-K$39)</f>
-        <v>0.15527950310559008</v>
+        <v>0.28735632183908044</v>
       </c>
       <c r="L34" s="1"/>
     </row>
@@ -1674,9 +1674,9 @@
       </c>
       <c r="C35" s="7">
         <f>C6/(1-C$39)</f>
-        <v>0.19183337900794736</v>
-      </c>
-      <c r="D35" s="34"/>
+        <v>0.36668412781561022</v>
+      </c>
+      <c r="D35" s="33"/>
       <c r="E35" s="7"/>
       <c r="F35" s="7">
         <f>F6/(1-F$39)</f>
@@ -1691,7 +1691,7 @@
       </c>
       <c r="K35" s="7">
         <f>K6/(1-K$39)</f>
-        <v>0.74534161490683237</v>
+        <v>0.68965517241379304</v>
       </c>
       <c r="L35" s="1"/>
     </row>
@@ -1700,10 +1700,10 @@
         <v>3</v>
       </c>
       <c r="C36" s="22"/>
-      <c r="D36" s="35"/>
+      <c r="D36" s="34"/>
       <c r="E36" s="22">
         <f>E7/(1-E$39)</f>
-        <v>0.79715302491103202</v>
+        <v>0.73587385019710894</v>
       </c>
       <c r="F36" s="22"/>
       <c r="G36" s="22"/>
@@ -1721,13 +1721,13 @@
         <v>4</v>
       </c>
       <c r="C37" s="7"/>
-      <c r="D37" s="34">
+      <c r="D37" s="33">
         <f>D8/(1-D$39)</f>
-        <v>0.83333333333333337</v>
+        <v>0.7142857142857143</v>
       </c>
       <c r="E37" s="7">
         <f>E8/(1-E$39)</f>
-        <v>0.14234875444839859</v>
+        <v>0.26281208935611039</v>
       </c>
       <c r="F37" s="7"/>
       <c r="G37" s="7"/>
@@ -1742,7 +1742,7 @@
       </c>
       <c r="K37" s="7">
         <f>K8/(1-K$39)</f>
-        <v>0.15527950310559008</v>
+        <v>0.28735632183908044</v>
       </c>
       <c r="L37" s="1"/>
     </row>
@@ -1752,36 +1752,36 @@
       </c>
       <c r="C38" s="22">
         <f>C29/(1-C$39)</f>
-        <v>0.38366675801589473</v>
-      </c>
-      <c r="D38" s="35"/>
+        <v>0.36668412781561022</v>
+      </c>
+      <c r="D38" s="34"/>
       <c r="E38" s="22">
-        <f>E29/(1-E$39)</f>
-        <v>0.39857651245551601</v>
+        <f t="shared" ref="E38:K38" si="1">E29/(1-E$39)</f>
+        <v>0.36793692509855447</v>
       </c>
       <c r="F38" s="22">
-        <f>F29/(1-F$39)</f>
+        <f t="shared" si="1"/>
         <v>0.35</v>
       </c>
       <c r="G38" s="22">
-        <f>G29/(1-G$39)</f>
+        <f t="shared" si="1"/>
         <v>0.35</v>
       </c>
       <c r="H38" s="22">
-        <f>H29/(1-H$39)</f>
+        <f t="shared" si="1"/>
         <v>0.4053271569195136</v>
       </c>
       <c r="I38" s="22">
-        <f>I29/(1-I$39)</f>
+        <f t="shared" si="1"/>
         <v>0.36668412781561022</v>
       </c>
       <c r="J38" s="22">
-        <f>J29/(1-J$39)</f>
+        <f t="shared" si="1"/>
         <v>0.43478260869565216</v>
       </c>
       <c r="K38" s="22">
-        <f>K29/(1-K$39)</f>
-        <v>0.43478260869565216</v>
+        <f t="shared" si="1"/>
+        <v>0.4022988505747126</v>
       </c>
       <c r="L38" s="10"/>
     </row>
@@ -1791,15 +1791,15 @@
       </c>
       <c r="C39" s="11">
         <f>C19*(1-C29)</f>
-        <v>8.7749999999999995E-2</v>
+        <v>4.5499999999999985E-2</v>
       </c>
       <c r="D39" s="11">
         <f>(1-D4-D5)*(1-D8)</f>
-        <v>0.27999999999999997</v>
+        <v>0.16000000000000003</v>
       </c>
       <c r="E39" s="11">
         <f>E19*(1-E29)</f>
-        <v>0.12187500000000002</v>
+        <v>4.8750000000000009E-2</v>
       </c>
       <c r="F39" s="11">
         <f>F19*(1-F29)</f>
@@ -1810,20 +1810,20 @@
         <v>0</v>
       </c>
       <c r="H39" s="11">
-        <f t="shared" ref="H39:K39" si="1">H19*(1-H29)</f>
+        <f t="shared" ref="H39:K39" si="2">H19*(1-H29)</f>
         <v>0.13650000000000001</v>
       </c>
       <c r="I39" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4.5499999999999985E-2</v>
       </c>
       <c r="J39" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.19500000000000003</v>
       </c>
       <c r="K39" s="11">
-        <f t="shared" si="1"/>
-        <v>0.19500000000000003</v>
+        <f t="shared" si="2"/>
+        <v>0.13</v>
       </c>
       <c r="L39" s="1"/>
       <c r="M39" t="s">
@@ -1836,39 +1836,39 @@
       </c>
       <c r="C40" s="24">
         <f>SUM(C33:C38)</f>
-        <v>1.6168813373526993</v>
-      </c>
-      <c r="D40" s="37">
-        <f t="shared" ref="D40:J40" si="2">SUM(D33:D38)</f>
-        <v>1.25</v>
+        <v>1.8858040859088527</v>
+      </c>
+      <c r="D40" s="36">
+        <f t="shared" ref="D40:J40" si="3">SUM(D33:D38)</f>
+        <v>1.4285714285714286</v>
       </c>
       <c r="E40" s="24">
-        <f t="shared" si="2"/>
-        <v>1.6227758007117439</v>
+        <f t="shared" si="3"/>
+        <v>1.8922470433639944</v>
       </c>
       <c r="F40" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.35</v>
       </c>
       <c r="G40" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.35</v>
       </c>
       <c r="H40" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.5634047481181239</v>
       </c>
       <c r="I40" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.6238868517548455</v>
       </c>
       <c r="J40" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.4906832298136645</v>
       </c>
       <c r="K40" s="24">
-        <f t="shared" ref="K40" si="3">SUM(K33:K38)</f>
-        <v>1.4906832298136645</v>
+        <f t="shared" ref="K40" si="4">SUM(K33:K38)</f>
+        <v>1.6666666666666665</v>
       </c>
       <c r="M40" t="s">
         <v>21</v>
@@ -2340,7 +2340,7 @@
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C45" s="27" t="s">
+      <c r="C45" s="41" t="s">
         <v>87</v>
       </c>
       <c r="D45" t="s">
@@ -2349,19 +2349,19 @@
       <c r="E45" t="s">
         <v>28</v>
       </c>
-      <c r="F45" s="27" t="s">
+      <c r="F45" s="41" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C46" s="27"/>
+      <c r="C46" s="41"/>
       <c r="D46" t="s">
         <v>80</v>
       </c>
       <c r="E46" t="s">
         <v>28</v>
       </c>
-      <c r="F46" s="27"/>
+      <c r="F46" s="41"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C47" t="s">

</xml_diff>

<commit_message>
Mise à jour du schéma d'attribution des ressources
Mise à jour suite au retrait de la pêche/pisci dans le reroll et aux
changements de valeurs
</commit_message>
<xml_diff>
--- a/Schémas.xlsx
+++ b/Schémas.xlsx
@@ -360,7 +360,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -382,6 +382,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -423,7 +429,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -529,6 +535,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -844,8 +853,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:U42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="I42" sqref="I42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -901,10 +910,12 @@
         <v>0.8</v>
       </c>
       <c r="D4" s="29">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
+      <c r="F4" s="6">
+        <v>0.1</v>
+      </c>
       <c r="G4" s="6">
         <v>1</v>
       </c>
@@ -926,13 +937,17 @@
         <v>0.3</v>
       </c>
       <c r="D5" s="30">
+        <v>0.2</v>
+      </c>
+      <c r="E5" s="20">
         <v>0.4</v>
       </c>
-      <c r="E5" s="20">
-        <v>0.5</v>
-      </c>
-      <c r="F5" s="20"/>
-      <c r="G5" s="20"/>
+      <c r="F5" s="20">
+        <v>0.05</v>
+      </c>
+      <c r="G5" s="20">
+        <v>0.1</v>
+      </c>
       <c r="H5" s="20"/>
       <c r="I5" s="20">
         <v>0.9</v>
@@ -954,11 +969,13 @@
       <c r="F6" s="6">
         <v>1</v>
       </c>
-      <c r="G6" s="6"/>
+      <c r="G6" s="6">
+        <v>0.05</v>
+      </c>
       <c r="H6" s="6"/>
       <c r="I6" s="5"/>
       <c r="J6" s="6">
-        <v>0.6</v>
+        <v>0.65</v>
       </c>
       <c r="K6" s="6">
         <v>0.6</v>
@@ -973,10 +990,14 @@
       <c r="E7" s="20">
         <v>0.7</v>
       </c>
-      <c r="F7" s="20"/>
-      <c r="G7" s="20"/>
+      <c r="F7" s="20">
+        <v>0.05</v>
+      </c>
+      <c r="G7" s="20">
+        <v>0.1</v>
+      </c>
       <c r="H7" s="20">
-        <v>0.3</v>
+        <v>0.25</v>
       </c>
       <c r="I7" s="21"/>
       <c r="J7" s="21"/>
@@ -989,22 +1010,26 @@
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="29">
-        <v>0.6</v>
+        <v>0.7</v>
       </c>
       <c r="E8" s="6">
         <v>0.25</v>
       </c>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
+      <c r="F8" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="G8" s="6">
+        <v>0.05</v>
+      </c>
       <c r="H8" s="6">
         <v>0.7</v>
       </c>
       <c r="I8" s="5"/>
       <c r="J8" s="6">
-        <v>0.25</v>
+        <v>0.3</v>
       </c>
       <c r="K8" s="6">
-        <v>0.25</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="9" spans="2:21" x14ac:dyDescent="0.25">
@@ -1117,10 +1142,13 @@
       </c>
       <c r="D13" s="33">
         <f>D4/(1-D$19)</f>
-        <v>0.22321428571428573</v>
+        <v>0.54945054945054939</v>
       </c>
       <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
+      <c r="F13" s="42">
+        <f>F4/(1-F$19)</f>
+        <v>0.1</v>
+      </c>
       <c r="G13" s="7">
         <f>G4/(1-G$19)</f>
         <v>1</v>
@@ -1152,14 +1180,20 @@
       </c>
       <c r="D14" s="34">
         <f>D5/(1-D$19)</f>
-        <v>0.44642857142857145</v>
+        <v>0.21978021978021978</v>
       </c>
       <c r="E14" s="22">
         <f>E5/(1-E$19)</f>
-        <v>0.54054054054054046</v>
-      </c>
-      <c r="F14" s="22"/>
-      <c r="G14" s="22"/>
+        <v>0.44692737430167601</v>
+      </c>
+      <c r="F14" s="22">
+        <f>F5/(1-F$19)</f>
+        <v>0.05</v>
+      </c>
+      <c r="G14" s="22">
+        <f t="shared" ref="G14:G18" si="0">G5/(1-G$19)</f>
+        <v>0.1</v>
+      </c>
       <c r="H14" s="22"/>
       <c r="I14" s="22">
         <f>I5/(1-I$19)</f>
@@ -1168,7 +1202,7 @@
       <c r="J14" s="22"/>
       <c r="K14" s="22">
         <f>K5/(1-K$19)</f>
-        <v>0.3125</v>
+        <v>0.32894736842105265</v>
       </c>
       <c r="M14" s="8"/>
       <c r="N14" s="8"/>
@@ -1194,16 +1228,19 @@
         <f>F6/(1-F$19)</f>
         <v>1</v>
       </c>
-      <c r="G15" s="7"/>
+      <c r="G15" s="7">
+        <f t="shared" si="0"/>
+        <v>0.05</v>
+      </c>
       <c r="H15" s="7"/>
       <c r="I15" s="7"/>
       <c r="J15" s="7">
         <f>J6/(1-J$19)</f>
-        <v>0.85714285714285721</v>
+        <v>0.86092715231788086</v>
       </c>
       <c r="K15" s="7">
         <f>K6/(1-K$19)</f>
-        <v>0.74999999999999989</v>
+        <v>0.78947368421052633</v>
       </c>
       <c r="M15" s="13"/>
       <c r="N15" s="13"/>
@@ -1223,13 +1260,19 @@
       <c r="D16" s="34"/>
       <c r="E16" s="22">
         <f>E7/(1-E$19)</f>
-        <v>0.75675675675675669</v>
-      </c>
-      <c r="F16" s="22"/>
-      <c r="G16" s="22"/>
+        <v>0.78212290502793291</v>
+      </c>
+      <c r="F16" s="22">
+        <f t="shared" ref="F16:F18" si="1">F7/(1-F$19)</f>
+        <v>0.05</v>
+      </c>
+      <c r="G16" s="22">
+        <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
       <c r="H16" s="22">
         <f>H7/(1-H$19)</f>
-        <v>0.37974683544303794</v>
+        <v>0.32258064516129037</v>
       </c>
       <c r="I16" s="22"/>
       <c r="J16" s="22"/>
@@ -1251,26 +1294,32 @@
       <c r="C17" s="7"/>
       <c r="D17" s="33">
         <f>D8/(1-D$19)</f>
-        <v>0.6696428571428571</v>
+        <v>0.76923076923076916</v>
       </c>
       <c r="E17" s="7">
         <f>E8/(1-E$19)</f>
-        <v>0.27027027027027023</v>
-      </c>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
+        <v>0.27932960893854747</v>
+      </c>
+      <c r="F17" s="7">
+        <f t="shared" si="1"/>
+        <v>0.1</v>
+      </c>
+      <c r="G17" s="7">
+        <f t="shared" si="0"/>
+        <v>0.05</v>
+      </c>
       <c r="H17" s="7">
         <f>H8/(1-H$19)</f>
-        <v>0.88607594936708856</v>
+        <v>0.90322580645161299</v>
       </c>
       <c r="I17" s="7"/>
       <c r="J17" s="7">
         <f>J8/(1-J$19)</f>
-        <v>0.35714285714285715</v>
+        <v>0.39735099337748342</v>
       </c>
       <c r="K17" s="7">
         <f>K8/(1-K$19)</f>
-        <v>0.3125</v>
+        <v>0.19736842105263158</v>
       </c>
       <c r="M17" s="8"/>
       <c r="N17" s="8"/>
@@ -1289,7 +1338,7 @@
       <c r="C18" s="22"/>
       <c r="D18" s="34">
         <f>D9/(1-D$19)</f>
-        <v>0.39062499999999994</v>
+        <v>0.38461538461538458</v>
       </c>
       <c r="E18" s="22"/>
       <c r="F18" s="22"/>
@@ -1317,24 +1366,24 @@
         <v>6.9999999999999979E-2</v>
       </c>
       <c r="D19" s="35">
-        <f>(1-D4-D5)*(1-D8)*(1-D9)</f>
-        <v>0.10400000000000002</v>
+        <f>(1-D4-D5)*(1-D8)</f>
+        <v>9.0000000000000011E-2</v>
       </c>
       <c r="E19" s="11">
         <f>(1-E7)*(1-E5-E8)</f>
-        <v>7.5000000000000011E-2</v>
+        <v>0.10500000000000001</v>
       </c>
       <c r="F19" s="11">
-        <f>(1-F6)</f>
+        <f>(1-F6)*(1-F4-F5-F7-F8)</f>
         <v>0</v>
       </c>
       <c r="G19" s="11">
-        <f>(1-G4)</f>
+        <f>(1-G4)*(1-G5-G6-G7-G8)</f>
         <v>0</v>
       </c>
       <c r="H19" s="11">
         <f>(1-H4)*(1-H5)*(1-H6)*(1-H7)*(1-H8)*(1-H9)</f>
-        <v>0.21000000000000002</v>
+        <v>0.22500000000000003</v>
       </c>
       <c r="I19" s="11">
         <f>(1-I4)*(1-I5)*(1-I6)*(1-I7)*(1-I8)*(1-I9)</f>
@@ -1342,11 +1391,11 @@
       </c>
       <c r="J19" s="11">
         <f>(1-J4)*(1-J5)*(1-J6)*(1-J7)*(1-J8)*(1-J9)</f>
-        <v>0.30000000000000004</v>
+        <v>0.24499999999999997</v>
       </c>
       <c r="K19" s="11">
         <f>(1-K6)*(1-K5-K8)</f>
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
       <c r="M19" t="s">
         <v>22</v>
@@ -1361,36 +1410,36 @@
         <v>1.5591397849462365</v>
       </c>
       <c r="D20" s="36">
-        <f t="shared" ref="D20:I20" si="0">SUM(D13:D18)</f>
-        <v>1.7299107142857144</v>
+        <f t="shared" ref="D20:I20" si="2">SUM(D13:D18)</f>
+        <v>1.9230769230769229</v>
       </c>
       <c r="E20" s="24">
-        <f t="shared" si="0"/>
-        <v>1.5675675675675673</v>
+        <f t="shared" si="2"/>
+        <v>1.5083798882681565</v>
       </c>
       <c r="F20" s="24">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f t="shared" si="2"/>
+        <v>1.3</v>
       </c>
       <c r="G20" s="24">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f t="shared" si="2"/>
+        <v>1.3000000000000003</v>
       </c>
       <c r="H20" s="24">
-        <f t="shared" si="0"/>
-        <v>1.2658227848101264</v>
+        <f t="shared" si="2"/>
+        <v>1.2258064516129035</v>
       </c>
       <c r="I20" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.2903225806451613</v>
       </c>
       <c r="J20" s="24">
         <f>SUM(J13:J18)</f>
-        <v>1.2142857142857144</v>
+        <v>1.2582781456953642</v>
       </c>
       <c r="K20" s="24">
         <f>SUM(K13:K18)</f>
-        <v>1.375</v>
+        <v>1.3157894736842106</v>
       </c>
       <c r="M20" t="s">
         <v>21</v>
@@ -1527,31 +1576,31 @@
         <v>14</v>
       </c>
       <c r="C29" s="20">
-        <v>0.35</v>
+        <v>0.3</v>
       </c>
       <c r="D29" s="30">
-        <v>0.35</v>
+        <v>0.3</v>
       </c>
       <c r="E29" s="20">
-        <v>0.35</v>
+        <v>0.3</v>
       </c>
       <c r="F29" s="20">
-        <v>0.35</v>
+        <v>0.3</v>
       </c>
       <c r="G29" s="20">
-        <v>0.35</v>
+        <v>0.3</v>
       </c>
       <c r="H29" s="20">
-        <v>0.35</v>
+        <v>0.3</v>
       </c>
       <c r="I29" s="20">
-        <v>0.35</v>
+        <v>0.3</v>
       </c>
       <c r="J29" s="20">
-        <v>0.35</v>
+        <v>0.3</v>
       </c>
       <c r="K29" s="20">
-        <v>0.35</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="30" spans="2:21" x14ac:dyDescent="0.25">
@@ -1617,14 +1666,17 @@
       </c>
       <c r="C33" s="7">
         <f>C4/(1-C$39)</f>
-        <v>0.83813514929282351</v>
+        <v>0.86021505376344087</v>
       </c>
       <c r="D33" s="33">
         <f>D4/(1-D$39)</f>
-        <v>0.23809523809523811</v>
+        <v>0.54945054945054939</v>
       </c>
       <c r="E33" s="7"/>
-      <c r="F33" s="7"/>
+      <c r="F33" s="7">
+        <f t="shared" ref="F33:G34" si="3">F4/(1-F$39)</f>
+        <v>0.1</v>
+      </c>
       <c r="G33" s="7">
         <f>G4/(1-G$39)</f>
         <v>1</v>
@@ -1632,7 +1684,7 @@
       <c r="H33" s="7"/>
       <c r="I33" s="7">
         <f>I4/(1-I$39)</f>
-        <v>0.31430068098480879</v>
+        <v>0.32258064516129031</v>
       </c>
       <c r="J33" s="7"/>
       <c r="K33" s="7"/>
@@ -1644,27 +1696,33 @@
       </c>
       <c r="C34" s="22">
         <f>C5/(1-C$39)</f>
-        <v>0.31430068098480879</v>
+        <v>0.32258064516129031</v>
       </c>
       <c r="D34" s="34">
         <f>D5/(1-D$39)</f>
-        <v>0.47619047619047622</v>
+        <v>0.21978021978021978</v>
       </c>
       <c r="E34" s="22">
         <f>E5/(1-E$39)</f>
-        <v>0.52562417871222078</v>
-      </c>
-      <c r="F34" s="22"/>
-      <c r="G34" s="22"/>
+        <v>0.44692737430167601</v>
+      </c>
+      <c r="F34" s="22">
+        <f t="shared" si="3"/>
+        <v>0.05</v>
+      </c>
+      <c r="G34" s="22">
+        <f t="shared" si="3"/>
+        <v>0.1</v>
+      </c>
       <c r="H34" s="22"/>
       <c r="I34" s="22">
         <f>I5/(1-I$39)</f>
-        <v>0.94290204295442637</v>
+        <v>0.96774193548387089</v>
       </c>
       <c r="J34" s="22"/>
       <c r="K34" s="22">
         <f>K5/(1-K$39)</f>
-        <v>0.28735632183908044</v>
+        <v>0.32894736842105265</v>
       </c>
       <c r="L34" s="1"/>
     </row>
@@ -1674,7 +1732,7 @@
       </c>
       <c r="C35" s="7">
         <f>C6/(1-C$39)</f>
-        <v>0.36668412781561022</v>
+        <v>0.37634408602150532</v>
       </c>
       <c r="D35" s="33"/>
       <c r="E35" s="7"/>
@@ -1682,16 +1740,19 @@
         <f>F6/(1-F$39)</f>
         <v>1</v>
       </c>
-      <c r="G35" s="7"/>
+      <c r="G35" s="7">
+        <f t="shared" ref="G35:G37" si="4">G6/(1-G$39)</f>
+        <v>0.05</v>
+      </c>
       <c r="H35" s="7"/>
       <c r="I35" s="7"/>
       <c r="J35" s="7">
         <f>J6/(1-J$39)</f>
-        <v>0.74534161490683237</v>
+        <v>0.86092715231788086</v>
       </c>
       <c r="K35" s="7">
         <f>K6/(1-K$39)</f>
-        <v>0.68965517241379304</v>
+        <v>0.78947368421052633</v>
       </c>
       <c r="L35" s="1"/>
     </row>
@@ -1703,13 +1764,19 @@
       <c r="D36" s="34"/>
       <c r="E36" s="22">
         <f>E7/(1-E$39)</f>
-        <v>0.73587385019710894</v>
-      </c>
-      <c r="F36" s="22"/>
-      <c r="G36" s="22"/>
+        <v>0.78212290502793291</v>
+      </c>
+      <c r="F36" s="22">
+        <f t="shared" ref="F36:F37" si="5">F7/(1-F$39)</f>
+        <v>0.05</v>
+      </c>
+      <c r="G36" s="22">
+        <f t="shared" si="4"/>
+        <v>0.1</v>
+      </c>
       <c r="H36" s="22">
         <f>H7/(1-H$39)</f>
-        <v>0.34742327735958312</v>
+        <v>0.32258064516129037</v>
       </c>
       <c r="I36" s="22"/>
       <c r="J36" s="22"/>
@@ -1723,26 +1790,32 @@
       <c r="C37" s="7"/>
       <c r="D37" s="33">
         <f>D8/(1-D$39)</f>
-        <v>0.7142857142857143</v>
+        <v>0.76923076923076916</v>
       </c>
       <c r="E37" s="7">
         <f>E8/(1-E$39)</f>
-        <v>0.26281208935611039</v>
-      </c>
-      <c r="F37" s="7"/>
-      <c r="G37" s="7"/>
+        <v>0.27932960893854747</v>
+      </c>
+      <c r="F37" s="7">
+        <f t="shared" si="5"/>
+        <v>0.1</v>
+      </c>
+      <c r="G37" s="7">
+        <f t="shared" si="4"/>
+        <v>0.05</v>
+      </c>
       <c r="H37" s="7">
         <f>H8/(1-H$39)</f>
-        <v>0.8106543138390272</v>
+        <v>0.90322580645161299</v>
       </c>
       <c r="I37" s="7"/>
       <c r="J37" s="7">
         <f>J8/(1-J$39)</f>
-        <v>0.31055900621118016</v>
+        <v>0.39735099337748342</v>
       </c>
       <c r="K37" s="7">
         <f>K8/(1-K$39)</f>
-        <v>0.28735632183908044</v>
+        <v>0.19736842105263158</v>
       </c>
       <c r="L37" s="1"/>
     </row>
@@ -1752,36 +1825,36 @@
       </c>
       <c r="C38" s="22">
         <f>C29/(1-C$39)</f>
-        <v>0.36668412781561022</v>
+        <v>0.32258064516129031</v>
       </c>
       <c r="D38" s="34"/>
       <c r="E38" s="22">
-        <f t="shared" ref="E38:K38" si="1">E29/(1-E$39)</f>
-        <v>0.36793692509855447</v>
+        <f t="shared" ref="E38:K38" si="6">E29/(1-E$39)</f>
+        <v>0.33519553072625696</v>
       </c>
       <c r="F38" s="22">
-        <f t="shared" si="1"/>
-        <v>0.35</v>
+        <f t="shared" si="6"/>
+        <v>0.3</v>
       </c>
       <c r="G38" s="22">
-        <f t="shared" si="1"/>
-        <v>0.35</v>
+        <f t="shared" si="6"/>
+        <v>0.3</v>
       </c>
       <c r="H38" s="22">
-        <f t="shared" si="1"/>
-        <v>0.4053271569195136</v>
+        <f t="shared" si="6"/>
+        <v>0.38709677419354843</v>
       </c>
       <c r="I38" s="22">
-        <f t="shared" si="1"/>
-        <v>0.36668412781561022</v>
+        <f t="shared" si="6"/>
+        <v>0.32258064516129031</v>
       </c>
       <c r="J38" s="22">
-        <f t="shared" si="1"/>
-        <v>0.43478260869565216</v>
+        <f t="shared" si="6"/>
+        <v>0.39735099337748342</v>
       </c>
       <c r="K38" s="22">
-        <f t="shared" si="1"/>
-        <v>0.4022988505747126</v>
+        <f t="shared" si="6"/>
+        <v>0.39473684210526316</v>
       </c>
       <c r="L38" s="10"/>
     </row>
@@ -1790,40 +1863,40 @@
         <v>13</v>
       </c>
       <c r="C39" s="11">
-        <f>C19*(1-C29)</f>
-        <v>4.5499999999999985E-2</v>
+        <f>C19</f>
+        <v>6.9999999999999979E-2</v>
       </c>
       <c r="D39" s="11">
-        <f>(1-D4-D5)*(1-D8)</f>
-        <v>0.16000000000000003</v>
+        <f t="shared" ref="D39:K39" si="7">D19</f>
+        <v>9.0000000000000011E-2</v>
       </c>
       <c r="E39" s="11">
-        <f>E19*(1-E29)</f>
-        <v>4.8750000000000009E-2</v>
+        <f t="shared" si="7"/>
+        <v>0.10500000000000001</v>
       </c>
       <c r="F39" s="11">
-        <f>F19*(1-F29)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="G39" s="11">
-        <f>G19*(1-G29)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H39" s="11">
-        <f t="shared" ref="H39:K39" si="2">H19*(1-H29)</f>
-        <v>0.13650000000000001</v>
+        <f t="shared" si="7"/>
+        <v>0.22500000000000003</v>
       </c>
       <c r="I39" s="11">
-        <f t="shared" si="2"/>
-        <v>4.5499999999999985E-2</v>
+        <f t="shared" si="7"/>
+        <v>6.9999999999999979E-2</v>
       </c>
       <c r="J39" s="11">
-        <f t="shared" si="2"/>
-        <v>0.19500000000000003</v>
+        <f t="shared" si="7"/>
+        <v>0.24499999999999997</v>
       </c>
       <c r="K39" s="11">
-        <f t="shared" si="2"/>
-        <v>0.13</v>
+        <f t="shared" si="7"/>
+        <v>0.24</v>
       </c>
       <c r="L39" s="1"/>
       <c r="M39" t="s">
@@ -1836,39 +1909,39 @@
       </c>
       <c r="C40" s="24">
         <f>SUM(C33:C38)</f>
-        <v>1.8858040859088527</v>
+        <v>1.8817204301075268</v>
       </c>
       <c r="D40" s="36">
-        <f t="shared" ref="D40:J40" si="3">SUM(D33:D38)</f>
-        <v>1.4285714285714286</v>
+        <f t="shared" ref="D40:J40" si="8">SUM(D33:D38)</f>
+        <v>1.5384615384615383</v>
       </c>
       <c r="E40" s="24">
-        <f t="shared" si="3"/>
-        <v>1.8922470433639944</v>
+        <f t="shared" si="8"/>
+        <v>1.8435754189944134</v>
       </c>
       <c r="F40" s="24">
-        <f t="shared" si="3"/>
-        <v>1.35</v>
+        <f t="shared" si="8"/>
+        <v>1.6</v>
       </c>
       <c r="G40" s="24">
-        <f t="shared" si="3"/>
-        <v>1.35</v>
+        <f t="shared" si="8"/>
+        <v>1.6000000000000003</v>
       </c>
       <c r="H40" s="24">
-        <f t="shared" si="3"/>
-        <v>1.5634047481181239</v>
+        <f t="shared" si="8"/>
+        <v>1.612903225806452</v>
       </c>
       <c r="I40" s="24">
-        <f t="shared" si="3"/>
-        <v>1.6238868517548455</v>
+        <f t="shared" si="8"/>
+        <v>1.6129032258064515</v>
       </c>
       <c r="J40" s="24">
-        <f t="shared" si="3"/>
-        <v>1.4906832298136645</v>
+        <f t="shared" si="8"/>
+        <v>1.6556291390728477</v>
       </c>
       <c r="K40" s="24">
-        <f t="shared" ref="K40" si="4">SUM(K33:K38)</f>
-        <v>1.6666666666666665</v>
+        <f t="shared" ref="K40" si="9">SUM(K33:K38)</f>
+        <v>1.7105263157894739</v>
       </c>
       <c r="M40" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
Analyse le décompte des ressources
Ajoute un nouvel onglet à la feuille excel pour analyser le comptage des
ressources de la province et de ses voisines
</commit_message>
<xml_diff>
--- a/Schémas.xlsx
+++ b/Schémas.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Ressources" sheetId="1" r:id="rId1"/>
-    <sheet name="Batiments" sheetId="2" r:id="rId2"/>
+    <sheet name="Spécialisation domaine" sheetId="3" r:id="rId2"/>
+    <sheet name="Batiments" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="109">
   <si>
     <t>Agriculture</t>
   </si>
@@ -310,13 +311,55 @@
   </si>
   <si>
     <t>Arctique</t>
+  </si>
+  <si>
+    <t>Nombre de provinces</t>
+  </si>
+  <si>
+    <t>20 ou +</t>
+  </si>
+  <si>
+    <t>Nombre de ressources</t>
+  </si>
+  <si>
+    <t>Ressources dans les provinces et leurs voisines (relevées sur une partie avec la carte Vanille en 2.4.4)</t>
+  </si>
+  <si>
+    <t>Provinces ayant au moins X ressources</t>
+  </si>
+  <si>
+    <t>Provinces ayant au plus X ressources</t>
+  </si>
+  <si>
+    <t>WARNING : Dans Notepad++, pensez à cocher mots entiers avant de faire compter</t>
+  </si>
+  <si>
+    <t>On peut découper cette répartition en 5 intervalles qui donneront des probas pour la spécialisation</t>
+  </si>
+  <si>
+    <t>7 à 8</t>
+  </si>
+  <si>
+    <t>1 à 6</t>
+  </si>
+  <si>
+    <t>10 à 11</t>
+  </si>
+  <si>
+    <t>12 et plus</t>
+  </si>
+  <si>
+    <t>Répartition sur l'exemple</t>
+  </si>
+  <si>
+    <t>Production</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -355,6 +398,30 @@
     <font>
       <b/>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -429,7 +496,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -533,10 +600,26 @@
     <xf numFmtId="9" fontId="4" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="16" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -586,6 +669,1153 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1500" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="100" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="fr-FR"/>
+              <a:t>Nombres de</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="fr-FR" baseline="0"/>
+              <a:t> RESSOURCES DANS LES POVINCES ET LEURS VOISINES</a:t>
+            </a:r>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1500" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="100" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw dist="25400" dir="2700000" algn="tl" rotWithShape="0">
+                <a:schemeClr val="accent1"/>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="fr-FR"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent1">
+                          <a:lumMod val="60000"/>
+                          <a:lumOff val="40000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Spécialisation domaine'!$B$4:$B$23</c:f>
+              <c:strCache>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20 ou +</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Spécialisation domaine'!$C$4:$C$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>136</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>184</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>136</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="ctr"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:dropLines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:gradFill>
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="lt1"/>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="lt1">
+                      <a:alpha val="0"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:dropLines>
+        <c:smooth val="0"/>
+        <c:axId val="331565728"/>
+        <c:axId val="331569648"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="331565728"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-FR"/>
+                  <a:t>Nombre</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="fr-FR" baseline="0"/>
+                  <a:t> de ressources</a:t>
+                </a:r>
+                <a:endParaRPr lang="fr-FR"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="30" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="331569648"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="331569648"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-FR"/>
+                  <a:t>Nombre</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="fr-FR" baseline="0"/>
+                  <a:t> de provinces</a:t>
+                </a:r>
+                <a:endParaRPr lang="fr-FR"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="331565728"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="accent1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="238">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" spc="30" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <cs:styleClr val="auto"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltUpDiag">
+        <a:fgClr>
+          <a:schemeClr val="phClr"/>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltUpDiag">
+        <a:fgClr>
+          <a:schemeClr val="phClr"/>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+      <a:effectLst>
+        <a:outerShdw dist="25400" dir="2700000" algn="tl" rotWithShape="0">
+          <a:schemeClr val="phClr"/>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="14"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="35000"/>
+          <a:lumOff val="65000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="lt1"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="lt1">
+                <a:alpha val="0"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="25400">
+          <a:schemeClr val="lt1"/>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+            <a:tint val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1500" b="1" kern="1200" cap="all" spc="100" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="95000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>157162</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Graphique 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -853,7 +2083,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:U42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="I42" sqref="I42"/>
     </sheetView>
   </sheetViews>
@@ -1145,7 +2375,7 @@
         <v>0.54945054945054939</v>
       </c>
       <c r="E13" s="7"/>
-      <c r="F13" s="42">
+      <c r="F13" s="41">
         <f>F4/(1-F$19)</f>
         <v>0.1</v>
       </c>
@@ -1191,7 +2421,7 @@
         <v>0.05</v>
       </c>
       <c r="G14" s="22">
-        <f t="shared" ref="G14:G18" si="0">G5/(1-G$19)</f>
+        <f t="shared" ref="G14:G17" si="0">G5/(1-G$19)</f>
         <v>0.1</v>
       </c>
       <c r="H14" s="22"/>
@@ -1263,7 +2493,7 @@
         <v>0.78212290502793291</v>
       </c>
       <c r="F16" s="22">
-        <f t="shared" ref="F16:F18" si="1">F7/(1-F$19)</f>
+        <f t="shared" ref="F16:F17" si="1">F7/(1-F$19)</f>
         <v>0.05</v>
       </c>
       <c r="G16" s="22">
@@ -1969,10 +3199,456 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="22.7109375" customWidth="1"/>
+    <col min="3" max="3" width="23.5703125" customWidth="1"/>
+    <col min="4" max="4" width="36.42578125" customWidth="1"/>
+    <col min="5" max="5" width="42.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="44" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="5">
+        <v>1</v>
+      </c>
+      <c r="C4" s="5">
+        <v>2</v>
+      </c>
+      <c r="D4" s="5">
+        <f>C4</f>
+        <v>2</v>
+      </c>
+      <c r="E4" s="5">
+        <f t="shared" ref="E4:E21" si="0">E5+C4</f>
+        <v>1237</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="43">
+        <v>2</v>
+      </c>
+      <c r="C5" s="43">
+        <v>7</v>
+      </c>
+      <c r="D5" s="43">
+        <f>D4+C5</f>
+        <v>9</v>
+      </c>
+      <c r="E5" s="43">
+        <f t="shared" si="0"/>
+        <v>1235</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="5">
+        <v>3</v>
+      </c>
+      <c r="C6" s="5">
+        <v>14</v>
+      </c>
+      <c r="D6" s="45">
+        <f t="shared" ref="D6:D23" si="1">D5+C6</f>
+        <v>23</v>
+      </c>
+      <c r="E6" s="5">
+        <f t="shared" si="0"/>
+        <v>1228</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="43">
+        <v>4</v>
+      </c>
+      <c r="C7" s="43">
+        <v>37</v>
+      </c>
+      <c r="D7" s="43">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+      <c r="E7" s="43">
+        <f t="shared" si="0"/>
+        <v>1214</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="5">
+        <v>5</v>
+      </c>
+      <c r="C8" s="5">
+        <v>60</v>
+      </c>
+      <c r="D8" s="45">
+        <f t="shared" si="1"/>
+        <v>120</v>
+      </c>
+      <c r="E8" s="5">
+        <f t="shared" si="0"/>
+        <v>1177</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="43">
+        <v>6</v>
+      </c>
+      <c r="C9" s="43">
+        <v>98</v>
+      </c>
+      <c r="D9" s="43">
+        <f t="shared" si="1"/>
+        <v>218</v>
+      </c>
+      <c r="E9" s="43">
+        <f t="shared" si="0"/>
+        <v>1117</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="5">
+        <v>7</v>
+      </c>
+      <c r="C10" s="5">
+        <v>136</v>
+      </c>
+      <c r="D10" s="45">
+        <f t="shared" si="1"/>
+        <v>354</v>
+      </c>
+      <c r="E10" s="5">
+        <f t="shared" si="0"/>
+        <v>1019</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="43">
+        <v>8</v>
+      </c>
+      <c r="C11" s="43">
+        <v>184</v>
+      </c>
+      <c r="D11" s="43">
+        <f t="shared" si="1"/>
+        <v>538</v>
+      </c>
+      <c r="E11" s="43">
+        <f t="shared" si="0"/>
+        <v>883</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="5">
+        <v>9</v>
+      </c>
+      <c r="C12" s="5">
+        <v>220</v>
+      </c>
+      <c r="D12" s="45">
+        <f t="shared" si="1"/>
+        <v>758</v>
+      </c>
+      <c r="E12" s="5">
+        <f t="shared" si="0"/>
+        <v>699</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="43">
+        <v>10</v>
+      </c>
+      <c r="C13" s="43">
+        <v>170</v>
+      </c>
+      <c r="D13" s="43">
+        <f t="shared" si="1"/>
+        <v>928</v>
+      </c>
+      <c r="E13" s="43">
+        <f t="shared" si="0"/>
+        <v>479</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B14" s="5">
+        <v>11</v>
+      </c>
+      <c r="C14" s="5">
+        <v>136</v>
+      </c>
+      <c r="D14" s="45">
+        <f t="shared" si="1"/>
+        <v>1064</v>
+      </c>
+      <c r="E14" s="5">
+        <f t="shared" si="0"/>
+        <v>309</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B15" s="43">
+        <v>12</v>
+      </c>
+      <c r="C15" s="43">
+        <v>80</v>
+      </c>
+      <c r="D15" s="43">
+        <f t="shared" si="1"/>
+        <v>1144</v>
+      </c>
+      <c r="E15" s="43">
+        <f t="shared" si="0"/>
+        <v>173</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B16" s="5">
+        <v>13</v>
+      </c>
+      <c r="C16" s="5">
+        <v>39</v>
+      </c>
+      <c r="D16" s="45">
+        <f t="shared" si="1"/>
+        <v>1183</v>
+      </c>
+      <c r="E16" s="5">
+        <f t="shared" si="0"/>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="43">
+        <v>14</v>
+      </c>
+      <c r="C17" s="43">
+        <v>25</v>
+      </c>
+      <c r="D17" s="43">
+        <f t="shared" si="1"/>
+        <v>1208</v>
+      </c>
+      <c r="E17" s="43">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="5">
+        <v>15</v>
+      </c>
+      <c r="C18" s="5">
+        <v>15</v>
+      </c>
+      <c r="D18" s="45">
+        <f t="shared" si="1"/>
+        <v>1223</v>
+      </c>
+      <c r="E18" s="5">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="43">
+        <v>16</v>
+      </c>
+      <c r="C19" s="43">
+        <v>9</v>
+      </c>
+      <c r="D19" s="43">
+        <f t="shared" si="1"/>
+        <v>1232</v>
+      </c>
+      <c r="E19" s="43">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="5">
+        <v>17</v>
+      </c>
+      <c r="C20" s="5">
+        <v>2</v>
+      </c>
+      <c r="D20" s="45">
+        <f t="shared" si="1"/>
+        <v>1234</v>
+      </c>
+      <c r="E20" s="5">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B21" s="43">
+        <v>18</v>
+      </c>
+      <c r="C21" s="43">
+        <v>2</v>
+      </c>
+      <c r="D21" s="43">
+        <f t="shared" si="1"/>
+        <v>1236</v>
+      </c>
+      <c r="E21" s="43">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="5">
+        <v>19</v>
+      </c>
+      <c r="C22" s="5">
+        <v>1</v>
+      </c>
+      <c r="D22" s="45">
+        <f t="shared" si="1"/>
+        <v>1237</v>
+      </c>
+      <c r="E22" s="5">
+        <f>E23+C22</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="43" t="s">
+        <v>96</v>
+      </c>
+      <c r="C23" s="43">
+        <v>0</v>
+      </c>
+      <c r="D23" s="43">
+        <f t="shared" si="1"/>
+        <v>1237</v>
+      </c>
+      <c r="E23" s="43">
+        <f>C23</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="46" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A27" s="48" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B28" s="4"/>
+      <c r="C28" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="E28" s="1"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B29" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="C29" s="5">
+        <f>D9</f>
+        <v>218</v>
+      </c>
+      <c r="D29" s="6">
+        <v>0.15</v>
+      </c>
+      <c r="E29" s="47"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B30" s="49" t="s">
+        <v>103</v>
+      </c>
+      <c r="C30" s="43">
+        <f>C10+C11</f>
+        <v>320</v>
+      </c>
+      <c r="D30" s="50">
+        <v>0.3</v>
+      </c>
+      <c r="E30" s="47"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B31" s="5">
+        <v>9</v>
+      </c>
+      <c r="C31" s="5">
+        <f>C12</f>
+        <v>220</v>
+      </c>
+      <c r="D31" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="E31" s="47"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B32" s="43" t="s">
+        <v>105</v>
+      </c>
+      <c r="C32" s="43">
+        <f>C13+C14</f>
+        <v>306</v>
+      </c>
+      <c r="D32" s="50">
+        <v>0.75</v>
+      </c>
+      <c r="E32" s="47"/>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B33" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="C33" s="5">
+        <f>E15</f>
+        <v>173</v>
+      </c>
+      <c r="D33" s="6">
+        <v>0.9</v>
+      </c>
+      <c r="E33" s="47"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C51" sqref="C51:F51"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2413,7 +4089,7 @@
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C45" s="41" t="s">
+      <c r="C45" s="42" t="s">
         <v>87</v>
       </c>
       <c r="D45" t="s">
@@ -2422,19 +4098,19 @@
       <c r="E45" t="s">
         <v>28</v>
       </c>
-      <c r="F45" s="41" t="s">
+      <c r="F45" s="42" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C46" s="41"/>
+      <c r="C46" s="42"/>
       <c r="D46" t="s">
         <v>80</v>
       </c>
       <c r="E46" t="s">
         <v>28</v>
       </c>
-      <c r="F46" s="41"/>
+      <c r="F46" s="42"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C47" t="s">

</xml_diff>

<commit_message>
Add a sheet on the iron productivity
Add some calculation in the spreadsheet, relative to the iron
consumption
</commit_message>
<xml_diff>
--- a/Schémas.xlsx
+++ b/Schémas.xlsx
@@ -13,8 +13,9 @@
   </bookViews>
   <sheets>
     <sheet name="Ressources" sheetId="1" r:id="rId1"/>
-    <sheet name="Spécialisation domaine" sheetId="3" r:id="rId2"/>
-    <sheet name="Batiments" sheetId="2" r:id="rId3"/>
+    <sheet name="Limitations" sheetId="4" r:id="rId2"/>
+    <sheet name="Spécialisation domaine" sheetId="3" r:id="rId3"/>
+    <sheet name="Batiments" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="120">
   <si>
     <t>Agriculture</t>
   </si>
@@ -353,13 +354,46 @@
   </si>
   <si>
     <t>Production</t>
+  </si>
+  <si>
+    <t>L1</t>
+  </si>
+  <si>
+    <t>L2</t>
+  </si>
+  <si>
+    <t>L3</t>
+  </si>
+  <si>
+    <t>Consommation</t>
+  </si>
+  <si>
+    <t>Accident</t>
+  </si>
+  <si>
+    <t>Hausse</t>
+  </si>
+  <si>
+    <t>Revenu</t>
+  </si>
+  <si>
+    <t>Revenu mensuel</t>
+  </si>
+  <si>
+    <t>Ratio</t>
+  </si>
+  <si>
+    <t>Base</t>
+  </si>
+  <si>
+    <t>PARAMETRES</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -426,8 +460,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -455,6 +496,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -496,7 +555,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -603,9 +662,6 @@
     <xf numFmtId="9" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -622,6 +678,23 @@
     <xf numFmtId="9" fontId="0" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -992,11 +1065,11 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="331565728"/>
-        <c:axId val="331569648"/>
+        <c:axId val="314982128"/>
+        <c:axId val="314983696"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="331565728"/>
+        <c:axId val="314982128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1085,7 +1158,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="331569648"/>
+        <c:crossAx val="314983696"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1093,7 +1166,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="331569648"/>
+        <c:axId val="314983696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1182,7 +1255,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="331565728"/>
+        <c:crossAx val="314982128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2083,8 +2156,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:U42"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="I42" sqref="I42"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3199,9 +3272,289 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.5703125" customWidth="1"/>
+    <col min="2" max="2" width="8.28515625" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="4" max="4" width="5.42578125" customWidth="1"/>
+    <col min="6" max="6" width="15" customWidth="1"/>
+    <col min="7" max="7" width="6" customWidth="1"/>
+    <col min="9" max="9" width="16.42578125" customWidth="1"/>
+    <col min="10" max="10" width="14.42578125" customWidth="1"/>
+    <col min="11" max="11" width="24.42578125" customWidth="1"/>
+    <col min="12" max="12" width="26" customWidth="1"/>
+    <col min="13" max="13" width="25.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="4"/>
+      <c r="B1" s="52" t="s">
+        <v>118</v>
+      </c>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="53" t="s">
+        <v>113</v>
+      </c>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="54" t="s">
+        <v>114</v>
+      </c>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="4"/>
+      <c r="B2" s="55" t="s">
+        <v>115</v>
+      </c>
+      <c r="C2" s="55" t="s">
+        <v>112</v>
+      </c>
+      <c r="D2" s="55" t="s">
+        <v>117</v>
+      </c>
+      <c r="E2" s="56" t="s">
+        <v>115</v>
+      </c>
+      <c r="F2" s="56" t="s">
+        <v>112</v>
+      </c>
+      <c r="G2" s="56" t="s">
+        <v>117</v>
+      </c>
+      <c r="H2" s="57" t="s">
+        <v>115</v>
+      </c>
+      <c r="I2" s="57" t="s">
+        <v>112</v>
+      </c>
+      <c r="J2" s="57" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B3" s="55">
+        <f>B9*12</f>
+        <v>1.2000000000000002</v>
+      </c>
+      <c r="C3" s="55">
+        <v>10</v>
+      </c>
+      <c r="D3" s="55">
+        <f>B3/C3</f>
+        <v>0.12000000000000002</v>
+      </c>
+      <c r="E3" s="56">
+        <f>B3*(1+C$15)</f>
+        <v>0.96000000000000019</v>
+      </c>
+      <c r="F3" s="56">
+        <f>C3*(1+C$14)</f>
+        <v>7</v>
+      </c>
+      <c r="G3" s="56">
+        <f>E3/F3</f>
+        <v>0.13714285714285718</v>
+      </c>
+      <c r="H3" s="57">
+        <f>B3*(1+C$19)</f>
+        <v>1.4400000000000002</v>
+      </c>
+      <c r="I3" s="57">
+        <f>C3*(1+C$18)</f>
+        <v>13</v>
+      </c>
+      <c r="J3" s="57">
+        <f>H3/I3</f>
+        <v>0.11076923076923079</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B4" s="55">
+        <f t="shared" ref="B4:B5" si="0">B10*12</f>
+        <v>2.4000000000000004</v>
+      </c>
+      <c r="C4" s="55">
+        <v>20</v>
+      </c>
+      <c r="D4" s="55">
+        <f t="shared" ref="D4:D5" si="1">B4/C4</f>
+        <v>0.12000000000000002</v>
+      </c>
+      <c r="E4" s="56">
+        <f t="shared" ref="E4:E5" si="2">B4*(1+C$15)</f>
+        <v>1.9200000000000004</v>
+      </c>
+      <c r="F4" s="56">
+        <f t="shared" ref="F4:F5" si="3">C4*(1+C$14)</f>
+        <v>14</v>
+      </c>
+      <c r="G4" s="56">
+        <f t="shared" ref="G4:G5" si="4">E4/F4</f>
+        <v>0.13714285714285718</v>
+      </c>
+      <c r="H4" s="57">
+        <f t="shared" ref="H4:H5" si="5">B4*(1+C$19)</f>
+        <v>2.8800000000000003</v>
+      </c>
+      <c r="I4" s="57">
+        <f t="shared" ref="I4:I5" si="6">C4*(1+C$18)</f>
+        <v>26</v>
+      </c>
+      <c r="J4" s="57">
+        <f t="shared" ref="J4:J5" si="7">H4/I4</f>
+        <v>0.11076923076923079</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="B5" s="55">
+        <f t="shared" si="0"/>
+        <v>3.5999999999999996</v>
+      </c>
+      <c r="C5" s="55">
+        <v>30</v>
+      </c>
+      <c r="D5" s="55">
+        <f t="shared" si="1"/>
+        <v>0.11999999999999998</v>
+      </c>
+      <c r="E5" s="56">
+        <f t="shared" si="2"/>
+        <v>2.88</v>
+      </c>
+      <c r="F5" s="58">
+        <v>20</v>
+      </c>
+      <c r="G5" s="56">
+        <f t="shared" si="4"/>
+        <v>0.14399999999999999</v>
+      </c>
+      <c r="H5" s="57">
+        <f t="shared" si="5"/>
+        <v>4.3199999999999994</v>
+      </c>
+      <c r="I5" s="58">
+        <v>40</v>
+      </c>
+      <c r="J5" s="57">
+        <f t="shared" si="7"/>
+        <v>0.10799999999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>119</v>
+      </c>
+      <c r="E7" s="46"/>
+      <c r="F7" s="46"/>
+      <c r="G7" s="46"/>
+      <c r="H7" s="51"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>109</v>
+      </c>
+      <c r="B9">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>110</v>
+      </c>
+      <c r="B10">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>111</v>
+      </c>
+      <c r="B11">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>112</v>
+      </c>
+      <c r="C14" s="2">
+        <v>-0.3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>115</v>
+      </c>
+      <c r="C15" s="46">
+        <v>-0.2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>112</v>
+      </c>
+      <c r="C18" s="2">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>115</v>
+      </c>
+      <c r="C19" s="46">
+        <v>0.2</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="H1:J1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
@@ -3214,7 +3567,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="43" t="s">
         <v>98</v>
       </c>
     </row>
@@ -3249,17 +3602,17 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="43">
+      <c r="B5" s="42">
         <v>2</v>
       </c>
-      <c r="C5" s="43">
+      <c r="C5" s="42">
         <v>7</v>
       </c>
-      <c r="D5" s="43">
+      <c r="D5" s="42">
         <f>D4+C5</f>
         <v>9</v>
       </c>
-      <c r="E5" s="43">
+      <c r="E5" s="42">
         <f t="shared" si="0"/>
         <v>1235</v>
       </c>
@@ -3271,7 +3624,7 @@
       <c r="C6" s="5">
         <v>14</v>
       </c>
-      <c r="D6" s="45">
+      <c r="D6" s="44">
         <f t="shared" ref="D6:D23" si="1">D5+C6</f>
         <v>23</v>
       </c>
@@ -3281,17 +3634,17 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="43">
+      <c r="B7" s="42">
         <v>4</v>
       </c>
-      <c r="C7" s="43">
+      <c r="C7" s="42">
         <v>37</v>
       </c>
-      <c r="D7" s="43">
+      <c r="D7" s="42">
         <f t="shared" si="1"/>
         <v>60</v>
       </c>
-      <c r="E7" s="43">
+      <c r="E7" s="42">
         <f t="shared" si="0"/>
         <v>1214</v>
       </c>
@@ -3303,7 +3656,7 @@
       <c r="C8" s="5">
         <v>60</v>
       </c>
-      <c r="D8" s="45">
+      <c r="D8" s="44">
         <f t="shared" si="1"/>
         <v>120</v>
       </c>
@@ -3313,17 +3666,17 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="43">
+      <c r="B9" s="42">
         <v>6</v>
       </c>
-      <c r="C9" s="43">
+      <c r="C9" s="42">
         <v>98</v>
       </c>
-      <c r="D9" s="43">
+      <c r="D9" s="42">
         <f t="shared" si="1"/>
         <v>218</v>
       </c>
-      <c r="E9" s="43">
+      <c r="E9" s="42">
         <f t="shared" si="0"/>
         <v>1117</v>
       </c>
@@ -3335,7 +3688,7 @@
       <c r="C10" s="5">
         <v>136</v>
       </c>
-      <c r="D10" s="45">
+      <c r="D10" s="44">
         <f t="shared" si="1"/>
         <v>354</v>
       </c>
@@ -3345,17 +3698,17 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="43">
+      <c r="B11" s="42">
         <v>8</v>
       </c>
-      <c r="C11" s="43">
+      <c r="C11" s="42">
         <v>184</v>
       </c>
-      <c r="D11" s="43">
+      <c r="D11" s="42">
         <f t="shared" si="1"/>
         <v>538</v>
       </c>
-      <c r="E11" s="43">
+      <c r="E11" s="42">
         <f t="shared" si="0"/>
         <v>883</v>
       </c>
@@ -3367,7 +3720,7 @@
       <c r="C12" s="5">
         <v>220</v>
       </c>
-      <c r="D12" s="45">
+      <c r="D12" s="44">
         <f t="shared" si="1"/>
         <v>758</v>
       </c>
@@ -3377,17 +3730,17 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="43">
+      <c r="B13" s="42">
         <v>10</v>
       </c>
-      <c r="C13" s="43">
+      <c r="C13" s="42">
         <v>170</v>
       </c>
-      <c r="D13" s="43">
+      <c r="D13" s="42">
         <f t="shared" si="1"/>
         <v>928</v>
       </c>
-      <c r="E13" s="43">
+      <c r="E13" s="42">
         <f t="shared" si="0"/>
         <v>479</v>
       </c>
@@ -3399,7 +3752,7 @@
       <c r="C14" s="5">
         <v>136</v>
       </c>
-      <c r="D14" s="45">
+      <c r="D14" s="44">
         <f t="shared" si="1"/>
         <v>1064</v>
       </c>
@@ -3409,17 +3762,17 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="43">
+      <c r="B15" s="42">
         <v>12</v>
       </c>
-      <c r="C15" s="43">
+      <c r="C15" s="42">
         <v>80</v>
       </c>
-      <c r="D15" s="43">
+      <c r="D15" s="42">
         <f t="shared" si="1"/>
         <v>1144</v>
       </c>
-      <c r="E15" s="43">
+      <c r="E15" s="42">
         <f t="shared" si="0"/>
         <v>173</v>
       </c>
@@ -3431,7 +3784,7 @@
       <c r="C16" s="5">
         <v>39</v>
       </c>
-      <c r="D16" s="45">
+      <c r="D16" s="44">
         <f t="shared" si="1"/>
         <v>1183</v>
       </c>
@@ -3441,17 +3794,17 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="43">
+      <c r="B17" s="42">
         <v>14</v>
       </c>
-      <c r="C17" s="43">
+      <c r="C17" s="42">
         <v>25</v>
       </c>
-      <c r="D17" s="43">
+      <c r="D17" s="42">
         <f t="shared" si="1"/>
         <v>1208</v>
       </c>
-      <c r="E17" s="43">
+      <c r="E17" s="42">
         <f t="shared" si="0"/>
         <v>54</v>
       </c>
@@ -3463,7 +3816,7 @@
       <c r="C18" s="5">
         <v>15</v>
       </c>
-      <c r="D18" s="45">
+      <c r="D18" s="44">
         <f t="shared" si="1"/>
         <v>1223</v>
       </c>
@@ -3473,17 +3826,17 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="43">
+      <c r="B19" s="42">
         <v>16</v>
       </c>
-      <c r="C19" s="43">
+      <c r="C19" s="42">
         <v>9</v>
       </c>
-      <c r="D19" s="43">
+      <c r="D19" s="42">
         <f t="shared" si="1"/>
         <v>1232</v>
       </c>
-      <c r="E19" s="43">
+      <c r="E19" s="42">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
@@ -3495,7 +3848,7 @@
       <c r="C20" s="5">
         <v>2</v>
       </c>
-      <c r="D20" s="45">
+      <c r="D20" s="44">
         <f t="shared" si="1"/>
         <v>1234</v>
       </c>
@@ -3505,17 +3858,17 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="43">
+      <c r="B21" s="42">
         <v>18</v>
       </c>
-      <c r="C21" s="43">
+      <c r="C21" s="42">
         <v>2</v>
       </c>
-      <c r="D21" s="43">
+      <c r="D21" s="42">
         <f t="shared" si="1"/>
         <v>1236</v>
       </c>
-      <c r="E21" s="43">
+      <c r="E21" s="42">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
@@ -3527,7 +3880,7 @@
       <c r="C22" s="5">
         <v>1</v>
       </c>
-      <c r="D22" s="45">
+      <c r="D22" s="44">
         <f t="shared" si="1"/>
         <v>1237</v>
       </c>
@@ -3537,28 +3890,28 @@
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B23" s="43" t="s">
+      <c r="B23" s="42" t="s">
         <v>96</v>
       </c>
-      <c r="C23" s="43">
+      <c r="C23" s="42">
         <v>0</v>
       </c>
-      <c r="D23" s="43">
+      <c r="D23" s="42">
         <f t="shared" si="1"/>
         <v>1237</v>
       </c>
-      <c r="E23" s="43">
+      <c r="E23" s="42">
         <f>C23</f>
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="46" t="s">
+      <c r="A25" s="45" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A27" s="48" t="s">
+      <c r="A27" s="47" t="s">
         <v>102</v>
       </c>
     </row>
@@ -3583,20 +3936,20 @@
       <c r="D29" s="6">
         <v>0.15</v>
       </c>
-      <c r="E29" s="47"/>
+      <c r="E29" s="46"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B30" s="49" t="s">
+      <c r="B30" s="48" t="s">
         <v>103</v>
       </c>
-      <c r="C30" s="43">
+      <c r="C30" s="42">
         <f>C10+C11</f>
         <v>320</v>
       </c>
-      <c r="D30" s="50">
+      <c r="D30" s="49">
         <v>0.3</v>
       </c>
-      <c r="E30" s="47"/>
+      <c r="E30" s="46"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B31" s="5">
@@ -3609,20 +3962,20 @@
       <c r="D31" s="6">
         <v>0.5</v>
       </c>
-      <c r="E31" s="47"/>
+      <c r="E31" s="46"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B32" s="43" t="s">
+      <c r="B32" s="42" t="s">
         <v>105</v>
       </c>
-      <c r="C32" s="43">
+      <c r="C32" s="42">
         <f>C13+C14</f>
         <v>306</v>
       </c>
-      <c r="D32" s="50">
+      <c r="D32" s="49">
         <v>0.75</v>
       </c>
-      <c r="E32" s="47"/>
+      <c r="E32" s="46"/>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
@@ -3635,7 +3988,7 @@
       <c r="D33" s="6">
         <v>0.9</v>
       </c>
-      <c r="E33" s="47"/>
+      <c r="E33" s="46"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3643,12 +3996,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="G40" sqref="G40"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4089,7 +4442,7 @@
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C45" s="42" t="s">
+      <c r="C45" s="50" t="s">
         <v>87</v>
       </c>
       <c r="D45" t="s">
@@ -4098,19 +4451,19 @@
       <c r="E45" t="s">
         <v>28</v>
       </c>
-      <c r="F45" s="42" t="s">
+      <c r="F45" s="50" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C46" s="42"/>
+      <c r="C46" s="50"/>
       <c r="D46" t="s">
         <v>80</v>
       </c>
       <c r="E46" t="s">
         <v>28</v>
       </c>
-      <c r="F46" s="42"/>
+      <c r="F46" s="50"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C47" t="s">

</xml_diff>

<commit_message>
Limit the iron mine to no desert province
Copper and gold are restricted to desert.
We wonder if it is a good idea to limit iron to non desert.
Like we remove the minerai1 modifier when there is no more ore, it is a
good idea to separate iron from copper and gold
</commit_message>
<xml_diff>
--- a/Schémas.xlsx
+++ b/Schémas.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="176">
   <si>
     <t>Agriculture</t>
   </si>
@@ -552,6 +552,9 @@
   </si>
   <si>
     <t>cidre (3)</t>
+  </si>
+  <si>
+    <t>Pas desert</t>
   </si>
 </sst>
 </file>
@@ -846,18 +849,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -875,32 +866,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Pourcentage" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -996,7 +979,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1087,7 +1069,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1275,11 +1256,11 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="152956544"/>
-        <c:axId val="105550200"/>
+        <c:axId val="152790360"/>
+        <c:axId val="152885512"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="152956544"/>
+        <c:axId val="152790360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1313,7 +1294,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1368,7 +1348,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="105550200"/>
+        <c:crossAx val="152885512"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1376,7 +1356,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="105550200"/>
+        <c:axId val="152885512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1410,7 +1390,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1465,7 +1444,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="152956544"/>
+        <c:crossAx val="152790360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3505,21 +3484,21 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
-      <c r="B1" s="54" t="s">
+      <c r="B1" s="61" t="s">
         <v>82</v>
       </c>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="55" t="s">
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="62" t="s">
         <v>77</v>
       </c>
-      <c r="F1" s="55"/>
-      <c r="G1" s="55"/>
-      <c r="H1" s="56" t="s">
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
+      <c r="H1" s="63" t="s">
         <v>78</v>
       </c>
-      <c r="I1" s="56"/>
-      <c r="J1" s="56"/>
+      <c r="I1" s="63"/>
+      <c r="J1" s="63"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
@@ -3718,7 +3697,7 @@
       <c r="A14" t="s">
         <v>76</v>
       </c>
-      <c r="C14" s="58">
+      <c r="C14" s="54">
         <v>-5</v>
       </c>
       <c r="D14" s="45"/>
@@ -3744,7 +3723,7 @@
       <c r="A18" t="s">
         <v>76</v>
       </c>
-      <c r="C18" s="58">
+      <c r="C18" s="54">
         <v>5</v>
       </c>
       <c r="D18" s="45"/>
@@ -4222,7 +4201,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4249,7 +4230,7 @@
       <c r="F2" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="G2" s="61" t="s">
+      <c r="G2" s="57" t="s">
         <v>85</v>
       </c>
       <c r="H2" t="s">
@@ -4260,7 +4241,7 @@
       <c r="C3" t="s">
         <v>86</v>
       </c>
-      <c r="D3" s="59" t="s">
+      <c r="D3" s="55" t="s">
         <v>87</v>
       </c>
       <c r="E3" t="s">
@@ -4269,7 +4250,7 @@
       <c r="F3" t="s">
         <v>89</v>
       </c>
-      <c r="G3" s="60" t="s">
+      <c r="G3" s="56" t="s">
         <v>92</v>
       </c>
     </row>
@@ -4311,7 +4292,7 @@
       <c r="C6" t="s">
         <v>93</v>
       </c>
-      <c r="D6" s="59" t="s">
+      <c r="D6" s="55" t="s">
         <v>87</v>
       </c>
       <c r="E6" t="s">
@@ -4328,7 +4309,7 @@
       <c r="C7" t="s">
         <v>100</v>
       </c>
-      <c r="D7" s="59" t="s">
+      <c r="D7" s="55" t="s">
         <v>102</v>
       </c>
       <c r="E7" t="s">
@@ -4345,7 +4326,7 @@
       <c r="C8" t="s">
         <v>99</v>
       </c>
-      <c r="D8" s="59" t="s">
+      <c r="D8" s="55" t="s">
         <v>102</v>
       </c>
       <c r="E8" t="s">
@@ -4362,7 +4343,7 @@
       <c r="C9" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="59" t="s">
+      <c r="D9" s="55" t="s">
         <v>102</v>
       </c>
       <c r="E9" t="s">
@@ -4405,7 +4386,7 @@
       <c r="F11" t="s">
         <v>109</v>
       </c>
-      <c r="G11" s="63" t="s">
+      <c r="G11" s="59" t="s">
         <v>113</v>
       </c>
     </row>
@@ -4440,7 +4421,7 @@
         <v>116</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>113</v>
+        <v>175</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -4503,7 +4484,7 @@
       <c r="C19" t="s">
         <v>124</v>
       </c>
-      <c r="D19" s="59" t="s">
+      <c r="D19" s="55" t="s">
         <v>87</v>
       </c>
       <c r="E19" t="s">
@@ -4512,7 +4493,7 @@
       <c r="F19" t="s">
         <v>89</v>
       </c>
-      <c r="G19" s="60" t="s">
+      <c r="G19" s="56" t="s">
         <v>92</v>
       </c>
     </row>
@@ -4554,7 +4535,7 @@
       <c r="C22" t="s">
         <v>125</v>
       </c>
-      <c r="D22" s="59" t="s">
+      <c r="D22" s="55" t="s">
         <v>87</v>
       </c>
       <c r="E22" t="s">
@@ -4571,7 +4552,7 @@
       <c r="C23" t="s">
         <v>126</v>
       </c>
-      <c r="D23" s="59" t="s">
+      <c r="D23" s="55" t="s">
         <v>102</v>
       </c>
       <c r="E23" t="s">
@@ -4631,7 +4612,7 @@
       <c r="F26" t="s">
         <v>109</v>
       </c>
-      <c r="G26" s="62" t="s">
+      <c r="G26" s="58" t="s">
         <v>129</v>
       </c>
     </row>
@@ -4752,7 +4733,7 @@
       <c r="C35" t="s">
         <v>141</v>
       </c>
-      <c r="D35" s="59" t="s">
+      <c r="D35" s="55" t="s">
         <v>87</v>
       </c>
       <c r="E35" t="s">
@@ -4761,7 +4742,7 @@
       <c r="F35" t="s">
         <v>89</v>
       </c>
-      <c r="G35" s="60" t="s">
+      <c r="G35" s="56" t="s">
         <v>92</v>
       </c>
     </row>
@@ -4812,7 +4793,7 @@
       <c r="F38" t="s">
         <v>151</v>
       </c>
-      <c r="G38" s="64" t="s">
+      <c r="G38" s="60" t="s">
         <v>113</v>
       </c>
       <c r="H38" s="45"/>
@@ -4821,7 +4802,7 @@
       <c r="C39" t="s">
         <v>146</v>
       </c>
-      <c r="D39" s="59" t="s">
+      <c r="D39" s="55" t="s">
         <v>87</v>
       </c>
       <c r="E39" t="s">
@@ -4855,7 +4836,7 @@
       <c r="C41" t="s">
         <v>142</v>
       </c>
-      <c r="D41" s="59" t="s">
+      <c r="D41" s="55" t="s">
         <v>87</v>
       </c>
       <c r="E41" t="s">
@@ -4875,7 +4856,7 @@
       <c r="C42" t="s">
         <v>152</v>
       </c>
-      <c r="D42" s="59" t="s">
+      <c r="D42" s="55" t="s">
         <v>102</v>
       </c>
       <c r="E42" t="s">
@@ -4901,7 +4882,7 @@
       <c r="F43" t="s">
         <v>109</v>
       </c>
-      <c r="G43" s="63" t="s">
+      <c r="G43" s="59" t="s">
         <v>113</v>
       </c>
     </row>
@@ -5101,7 +5082,7 @@
       <c r="F61" t="s">
         <v>151</v>
       </c>
-      <c r="G61" s="64"/>
+      <c r="G61" s="60"/>
     </row>
     <row r="62" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C62" t="s">
@@ -5116,7 +5097,7 @@
       <c r="F62" t="s">
         <v>149</v>
       </c>
-      <c r="G62" s="64"/>
+      <c r="G62" s="60"/>
       <c r="H62" s="45" t="s">
         <v>169</v>
       </c>
@@ -5192,26 +5173,26 @@
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C68" s="57" t="s">
+      <c r="C68" s="64" t="s">
         <v>52</v>
       </c>
       <c r="D68" t="s">
         <v>134</v>
       </c>
-      <c r="E68" s="57" t="s">
-        <v>27</v>
-      </c>
-      <c r="F68" s="57" t="s">
+      <c r="E68" s="64" t="s">
+        <v>27</v>
+      </c>
+      <c r="F68" s="64" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C69" s="57"/>
+      <c r="C69" s="64"/>
       <c r="D69" t="s">
         <v>128</v>
       </c>
-      <c r="E69" s="57"/>
-      <c r="F69" s="57"/>
+      <c r="E69" s="64"/>
+      <c r="F69" s="64"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
@@ -5253,12 +5234,12 @@
       <c r="A75" s="18"/>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C76" s="57"/>
-      <c r="F76" s="57"/>
+      <c r="C76" s="64"/>
+      <c r="F76" s="64"/>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C77" s="57"/>
-      <c r="F77" s="57"/>
+      <c r="C77" s="64"/>
+      <c r="F77" s="64"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>

<commit_message>
Duplicate minerai1 to have minerai1_sel
We need to separate the salt of the iron.
Like the salt is not restricted by province terrain, we needed to have a
new level 1 modifier: minerai1_sel
</commit_message>
<xml_diff>
--- a/Schémas.xlsx
+++ b/Schémas.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="177">
   <si>
     <t>Agriculture</t>
   </si>
@@ -555,6 +555,9 @@
   </si>
   <si>
     <t>Pas desert</t>
+  </si>
+  <si>
+    <t>minerai sel (1)</t>
   </si>
 </sst>
 </file>
@@ -1256,11 +1259,11 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="152790360"/>
-        <c:axId val="152885512"/>
+        <c:axId val="157480664"/>
+        <c:axId val="106053416"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="152790360"/>
+        <c:axId val="157480664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1348,7 +1351,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="152885512"/>
+        <c:crossAx val="106053416"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1356,7 +1359,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="152885512"/>
+        <c:axId val="106053416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1444,7 +1447,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="152790360"/>
+        <c:crossAx val="157480664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4201,8 +4204,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4638,7 +4641,7 @@
         <v>133</v>
       </c>
       <c r="D28" t="s">
-        <v>115</v>
+        <v>176</v>
       </c>
       <c r="E28" t="s">
         <v>27</v>

</xml_diff>

<commit_message>
Balance the tax income of the mine
The tax income wasn't balanced according to:
- ore consumption with the immersion events
- the initial cost of the buildings
</commit_message>
<xml_diff>
--- a/Schémas.xlsx
+++ b/Schémas.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Ressources" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="178">
   <si>
     <t>Agriculture</t>
   </si>
@@ -269,9 +269,6 @@
     <t>Revenu</t>
   </si>
   <si>
-    <t>Revenu mensuel</t>
-  </si>
-  <si>
     <t>Ratio</t>
   </si>
   <si>
@@ -281,9 +278,6 @@
     <t>PARAMETRES</t>
   </si>
   <si>
-    <t>Don't exist!</t>
-  </si>
-  <si>
     <t>TERRAIN</t>
   </si>
   <si>
@@ -558,6 +552,15 @@
   </si>
   <si>
     <t>minerai sel (1)</t>
+  </si>
+  <si>
+    <t>Coût construction</t>
+  </si>
+  <si>
+    <t>ROI années avant remboursement)</t>
+  </si>
+  <si>
+    <t>Revenu annuel</t>
   </si>
 </sst>
 </file>
@@ -725,7 +728,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -869,6 +872,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1259,11 +1263,11 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="157480664"/>
-        <c:axId val="106053416"/>
+        <c:axId val="153681376"/>
+        <c:axId val="151827064"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="157480664"/>
+        <c:axId val="153681376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1351,7 +1355,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="106053416"/>
+        <c:crossAx val="151827064"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1359,7 +1363,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="106053416"/>
+        <c:axId val="151827064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1447,7 +1451,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="157480664"/>
+        <c:crossAx val="153681376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3464,10 +3468,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3480,30 +3484,36 @@
     <col min="7" max="7" width="6" customWidth="1"/>
     <col min="9" max="9" width="16.42578125" customWidth="1"/>
     <col min="10" max="10" width="14.42578125" customWidth="1"/>
-    <col min="11" max="11" width="24.42578125" customWidth="1"/>
-    <col min="12" max="12" width="26" customWidth="1"/>
+    <col min="11" max="11" width="16.5703125" customWidth="1"/>
+    <col min="12" max="12" width="28.85546875" customWidth="1"/>
     <col min="13" max="13" width="25.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
-      <c r="B1" s="61" t="s">
-        <v>82</v>
-      </c>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="62" t="s">
+      <c r="B1" s="62" t="s">
+        <v>81</v>
+      </c>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="63" t="s">
         <v>77</v>
       </c>
-      <c r="F1" s="62"/>
-      <c r="G1" s="62"/>
-      <c r="H1" s="63" t="s">
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="64" t="s">
         <v>78</v>
       </c>
-      <c r="I1" s="63"/>
-      <c r="J1" s="63"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I1" s="64"/>
+      <c r="J1" s="64"/>
+      <c r="K1" t="s">
+        <v>175</v>
+      </c>
+      <c r="L1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="51" t="s">
         <v>79</v>
@@ -3512,7 +3522,7 @@
         <v>76</v>
       </c>
       <c r="D2" s="51" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E2" s="52" t="s">
         <v>79</v>
@@ -3521,7 +3531,7 @@
         <v>76</v>
       </c>
       <c r="G2" s="52" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H2" s="53" t="s">
         <v>79</v>
@@ -3530,27 +3540,27 @@
         <v>76</v>
       </c>
       <c r="J2" s="53" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>73</v>
       </c>
       <c r="B3" s="51">
-        <f>B9*12</f>
-        <v>1.2000000000000002</v>
+        <f>B9</f>
+        <v>0.2</v>
       </c>
       <c r="C3" s="51">
         <v>10</v>
       </c>
       <c r="D3" s="51">
         <f>B3/C3</f>
-        <v>0.12000000000000002</v>
+        <v>0.02</v>
       </c>
       <c r="E3" s="52">
-        <f>B3*(1+C$15)</f>
-        <v>1.2000000000000002</v>
+        <f>B3+C$15</f>
+        <v>0</v>
       </c>
       <c r="F3" s="52">
         <f>C3+C$14</f>
@@ -3558,11 +3568,11 @@
       </c>
       <c r="G3" s="52">
         <f>E3/F3</f>
-        <v>0.24000000000000005</v>
+        <v>0</v>
       </c>
       <c r="H3" s="53">
-        <f>B3*(1+C$19)</f>
-        <v>1.2000000000000002</v>
+        <f>B3+C$19</f>
+        <v>0.4</v>
       </c>
       <c r="I3" s="53">
         <f>C3+C$18</f>
@@ -3570,27 +3580,34 @@
       </c>
       <c r="J3" s="53">
         <f>H3/I3</f>
-        <v>8.0000000000000016E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+        <v>2.6666666666666668E-2</v>
+      </c>
+      <c r="K3">
+        <v>70</v>
+      </c>
+      <c r="L3">
+        <f>K3/B3</f>
+        <v>350</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>74</v>
       </c>
       <c r="B4" s="51">
-        <f t="shared" ref="B4:B5" si="0">B10*12</f>
-        <v>3.5999999999999996</v>
+        <f t="shared" ref="B4:B5" si="0">B10</f>
+        <v>0.4</v>
       </c>
       <c r="C4" s="51">
         <v>20</v>
       </c>
       <c r="D4" s="51">
         <f t="shared" ref="D4:D5" si="1">B4/C4</f>
-        <v>0.18</v>
+        <v>0.02</v>
       </c>
       <c r="E4" s="52">
-        <f t="shared" ref="E4:E5" si="2">B4*(1+C$15)</f>
-        <v>3.5999999999999996</v>
+        <f t="shared" ref="E4:E5" si="2">B4+C$15</f>
+        <v>0.2</v>
       </c>
       <c r="F4" s="52">
         <f t="shared" ref="F4:F5" si="3">C4+C$14</f>
@@ -3598,11 +3615,11 @@
       </c>
       <c r="G4" s="52">
         <f t="shared" ref="G4:G5" si="4">E4/F4</f>
-        <v>0.23999999999999996</v>
+        <v>1.3333333333333334E-2</v>
       </c>
       <c r="H4" s="53">
-        <f t="shared" ref="H4:H5" si="5">B4*(1+C$19)</f>
-        <v>3.5999999999999996</v>
+        <f t="shared" ref="H4:H5" si="5">B4+C$19</f>
+        <v>0.60000000000000009</v>
       </c>
       <c r="I4" s="53">
         <f t="shared" ref="I4:I5" si="6">C4+C$18</f>
@@ -3610,27 +3627,34 @@
       </c>
       <c r="J4" s="53">
         <f t="shared" ref="J4:J5" si="7">H4/I4</f>
-        <v>0.14399999999999999</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+        <v>2.4000000000000004E-2</v>
+      </c>
+      <c r="K4">
+        <v>105</v>
+      </c>
+      <c r="L4">
+        <f t="shared" ref="L4:L5" si="8">K4/B4</f>
+        <v>262.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>75</v>
       </c>
       <c r="B5" s="51">
         <f t="shared" si="0"/>
-        <v>4.8000000000000007</v>
+        <v>0.6</v>
       </c>
       <c r="C5" s="51">
         <v>30</v>
       </c>
       <c r="D5" s="51">
         <f t="shared" si="1"/>
-        <v>0.16000000000000003</v>
+        <v>0.02</v>
       </c>
       <c r="E5" s="52">
         <f t="shared" si="2"/>
-        <v>4.8000000000000007</v>
+        <v>0.39999999999999997</v>
       </c>
       <c r="F5" s="52">
         <f t="shared" si="3"/>
@@ -3638,11 +3662,11 @@
       </c>
       <c r="G5" s="52">
         <f t="shared" si="4"/>
-        <v>0.19200000000000003</v>
+        <v>1.6E-2</v>
       </c>
       <c r="H5" s="53">
         <f t="shared" si="5"/>
-        <v>4.8000000000000007</v>
+        <v>0.8</v>
       </c>
       <c r="I5" s="53">
         <f t="shared" si="6"/>
@@ -3650,53 +3674,60 @@
       </c>
       <c r="J5" s="53">
         <f t="shared" si="7"/>
-        <v>0.13714285714285715</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+        <v>2.2857142857142857E-2</v>
+      </c>
+      <c r="K5">
+        <v>200</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="8"/>
+        <v>333.33333333333337</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E7" s="46"/>
       <c r="F7" s="46"/>
       <c r="G7" s="46"/>
       <c r="H7" s="50"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>73</v>
       </c>
       <c r="B9">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>74</v>
       </c>
       <c r="B10">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>75</v>
       </c>
       <c r="B11">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>76</v>
       </c>
@@ -3706,16 +3737,14 @@
       <c r="D14" s="45"/>
       <c r="F14" s="45"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>79</v>
       </c>
-      <c r="C15" s="46">
-        <v>0</v>
-      </c>
-      <c r="D15" s="45" t="s">
-        <v>84</v>
-      </c>
+      <c r="C15" s="61">
+        <v>-0.2</v>
+      </c>
+      <c r="D15" s="45"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
@@ -3736,12 +3765,10 @@
       <c r="A19" t="s">
         <v>79</v>
       </c>
-      <c r="C19" s="46">
-        <v>0</v>
-      </c>
-      <c r="D19" s="45" t="s">
-        <v>84</v>
-      </c>
+      <c r="C19" s="61">
+        <v>0.2</v>
+      </c>
+      <c r="D19" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -4204,7 +4231,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+    <sheetView topLeftCell="A49" workbookViewId="0">
       <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
@@ -4228,33 +4255,33 @@
         <v>25</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G2" s="57" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D3" s="55" t="s">
+        <v>85</v>
+      </c>
+      <c r="E3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" t="s">
         <v>87</v>
       </c>
-      <c r="E3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F3" t="s">
-        <v>89</v>
-      </c>
       <c r="G3" s="56" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -4262,16 +4289,16 @@
         <v>26</v>
       </c>
       <c r="D4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E4" t="s">
         <v>27</v>
       </c>
       <c r="F4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -4279,64 +4306,64 @@
         <v>28</v>
       </c>
       <c r="D5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E5" t="s">
         <v>27</v>
       </c>
       <c r="F5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
+        <v>91</v>
+      </c>
+      <c r="D6" s="55" t="s">
+        <v>85</v>
+      </c>
+      <c r="E6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" t="s">
+        <v>92</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="D6" s="55" t="s">
-        <v>87</v>
-      </c>
-      <c r="E6" t="s">
-        <v>27</v>
-      </c>
-      <c r="F6" t="s">
-        <v>94</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
+        <v>98</v>
+      </c>
+      <c r="D7" s="55" t="s">
         <v>100</v>
       </c>
-      <c r="D7" s="55" t="s">
-        <v>102</v>
-      </c>
       <c r="E7" t="s">
         <v>27</v>
       </c>
       <c r="F7" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
+        <v>97</v>
+      </c>
+      <c r="D8" s="55" t="s">
+        <v>100</v>
+      </c>
+      <c r="E8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" t="s">
         <v>99</v>
-      </c>
-      <c r="D8" s="55" t="s">
-        <v>102</v>
-      </c>
-      <c r="E8" t="s">
-        <v>27</v>
-      </c>
-      <c r="F8" t="s">
-        <v>101</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>7</v>
@@ -4347,118 +4374,118 @@
         <v>30</v>
       </c>
       <c r="D9" s="55" t="s">
+        <v>100</v>
+      </c>
+      <c r="E9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" t="s">
+        <v>101</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>102</v>
-      </c>
-      <c r="E9" t="s">
-        <v>27</v>
-      </c>
-      <c r="F9" t="s">
-        <v>103</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
+        <v>103</v>
+      </c>
+      <c r="D10" t="s">
+        <v>104</v>
+      </c>
+      <c r="E10" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10" t="s">
         <v>105</v>
       </c>
-      <c r="D10" t="s">
-        <v>106</v>
-      </c>
-      <c r="E10" t="s">
-        <v>27</v>
-      </c>
-      <c r="F10" t="s">
-        <v>107</v>
-      </c>
       <c r="G10" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D11" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E11" t="s">
         <v>27</v>
       </c>
       <c r="F11" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G11" s="59" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
+        <v>108</v>
+      </c>
+      <c r="D12" t="s">
+        <v>109</v>
+      </c>
+      <c r="E12" t="s">
+        <v>27</v>
+      </c>
+      <c r="F12" t="s">
         <v>110</v>
       </c>
-      <c r="D12" t="s">
+      <c r="G12" s="1" t="s">
         <v>111</v>
-      </c>
-      <c r="E12" t="s">
-        <v>27</v>
-      </c>
-      <c r="F12" t="s">
-        <v>112</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
+        <v>112</v>
+      </c>
+      <c r="D13" t="s">
+        <v>113</v>
+      </c>
+      <c r="E13" t="s">
+        <v>27</v>
+      </c>
+      <c r="F13" t="s">
         <v>114</v>
       </c>
-      <c r="D13" t="s">
-        <v>115</v>
-      </c>
-      <c r="E13" t="s">
-        <v>27</v>
-      </c>
-      <c r="F13" t="s">
-        <v>116</v>
-      </c>
       <c r="G13" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
+        <v>115</v>
+      </c>
+      <c r="D14" t="s">
+        <v>116</v>
+      </c>
+      <c r="E14" t="s">
+        <v>27</v>
+      </c>
+      <c r="F14" t="s">
         <v>117</v>
       </c>
-      <c r="D14" t="s">
-        <v>118</v>
-      </c>
-      <c r="E14" t="s">
-        <v>27</v>
-      </c>
-      <c r="F14" t="s">
-        <v>119</v>
-      </c>
       <c r="G14" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D15" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E15" t="s">
         <v>27</v>
       </c>
       <c r="F15" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -4466,16 +4493,16 @@
         <v>29</v>
       </c>
       <c r="D16" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E16" t="s">
         <v>27</v>
       </c>
       <c r="F16" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
@@ -4485,19 +4512,19 @@
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D19" s="55" t="s">
+        <v>85</v>
+      </c>
+      <c r="E19" t="s">
+        <v>27</v>
+      </c>
+      <c r="F19" t="s">
         <v>87</v>
       </c>
-      <c r="E19" t="s">
-        <v>27</v>
-      </c>
-      <c r="F19" t="s">
-        <v>89</v>
-      </c>
       <c r="G19" s="56" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
@@ -4505,16 +4532,16 @@
         <v>36</v>
       </c>
       <c r="D20" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E20" t="s">
         <v>27</v>
       </c>
       <c r="F20" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
@@ -4522,50 +4549,50 @@
         <v>37</v>
       </c>
       <c r="D21" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E21" t="s">
         <v>27</v>
       </c>
       <c r="F21" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D22" s="55" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E22" t="s">
         <v>27</v>
       </c>
       <c r="F22" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D23" s="55" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E23" t="s">
         <v>27</v>
       </c>
       <c r="F23" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
@@ -4573,135 +4600,135 @@
         <v>32</v>
       </c>
       <c r="D24" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E24" t="s">
         <v>27</v>
       </c>
       <c r="F24" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D25" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E25" t="s">
         <v>27</v>
       </c>
       <c r="F25" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D26" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E26" t="s">
         <v>27</v>
       </c>
       <c r="F26" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G26" s="58" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D27" t="s">
+        <v>109</v>
+      </c>
+      <c r="E27" t="s">
+        <v>27</v>
+      </c>
+      <c r="F27" t="s">
+        <v>110</v>
+      </c>
+      <c r="G27" s="1" t="s">
         <v>111</v>
-      </c>
-      <c r="E27" t="s">
-        <v>27</v>
-      </c>
-      <c r="F27" t="s">
-        <v>112</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D28" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E28" t="s">
         <v>27</v>
       </c>
       <c r="F28" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D29" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E29" t="s">
         <v>27</v>
       </c>
       <c r="F29" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D30" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E30" t="s">
         <v>27</v>
       </c>
       <c r="F30" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D31" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E31" t="s">
         <v>27</v>
       </c>
       <c r="F31" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.25">
@@ -4709,19 +4736,19 @@
         <v>38</v>
       </c>
       <c r="D32" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E32" t="s">
         <v>27</v>
       </c>
       <c r="F32" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="H32" s="45" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -4734,19 +4761,19 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C35" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D35" s="55" t="s">
+        <v>85</v>
+      </c>
+      <c r="E35" t="s">
+        <v>27</v>
+      </c>
+      <c r="F35" t="s">
         <v>87</v>
       </c>
-      <c r="E35" t="s">
-        <v>27</v>
-      </c>
-      <c r="F35" t="s">
-        <v>89</v>
-      </c>
       <c r="G35" s="56" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
@@ -4754,16 +4781,16 @@
         <v>39</v>
       </c>
       <c r="D36" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E36" t="s">
         <v>27</v>
       </c>
       <c r="F36" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
@@ -4771,139 +4798,139 @@
         <v>40</v>
       </c>
       <c r="D37" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E37" t="s">
         <v>27</v>
       </c>
       <c r="F37" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C38" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D38" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E38" t="s">
         <v>27</v>
       </c>
       <c r="F38" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="G38" s="60" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="H38" s="45"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C39" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D39" s="55" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E39" t="s">
         <v>27</v>
       </c>
       <c r="F39" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C40" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D40" t="s">
+        <v>145</v>
+      </c>
+      <c r="E40" t="s">
+        <v>27</v>
+      </c>
+      <c r="F40" t="s">
         <v>147</v>
       </c>
-      <c r="E40" t="s">
-        <v>27</v>
-      </c>
-      <c r="F40" t="s">
-        <v>149</v>
-      </c>
       <c r="G40" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C41" t="s">
+        <v>140</v>
+      </c>
+      <c r="D41" s="55" t="s">
+        <v>85</v>
+      </c>
+      <c r="E41" t="s">
+        <v>27</v>
+      </c>
+      <c r="F41" t="s">
         <v>142</v>
-      </c>
-      <c r="D41" s="55" t="s">
-        <v>87</v>
-      </c>
-      <c r="E41" t="s">
-        <v>27</v>
-      </c>
-      <c r="F41" t="s">
-        <v>144</v>
       </c>
       <c r="G41" s="1" t="s">
         <v>5</v>
       </c>
       <c r="H41" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C42" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D42" s="55" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E42" t="s">
         <v>27</v>
       </c>
       <c r="F42" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C43" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D43" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E43" t="s">
         <v>27</v>
       </c>
       <c r="F43" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G43" s="59" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C44" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D44" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E44" t="s">
         <v>27</v>
       </c>
       <c r="F44" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
@@ -4911,19 +4938,19 @@
         <v>41</v>
       </c>
       <c r="D45" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E45" t="s">
         <v>27</v>
       </c>
       <c r="F45" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="H45" s="45" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
@@ -4936,13 +4963,13 @@
         <v>25</v>
       </c>
       <c r="D48" s="18" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F48" s="18" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G48" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.25">
@@ -4950,13 +4977,13 @@
         <v>42</v>
       </c>
       <c r="D49" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E49" t="s">
         <v>27</v>
       </c>
       <c r="F49" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="50" spans="2:8" x14ac:dyDescent="0.25">
@@ -4964,13 +4991,13 @@
         <v>43</v>
       </c>
       <c r="D50" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E50" t="s">
         <v>27</v>
       </c>
       <c r="F50" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="51" spans="2:8" x14ac:dyDescent="0.25">
@@ -4978,13 +5005,13 @@
         <v>44</v>
       </c>
       <c r="D51" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E51" t="s">
         <v>27</v>
       </c>
       <c r="F51" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="52" spans="2:8" x14ac:dyDescent="0.25">
@@ -4992,18 +5019,18 @@
         <v>45</v>
       </c>
       <c r="D52" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E52" t="s">
         <v>27</v>
       </c>
       <c r="F52" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="53" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="54" spans="2:8" x14ac:dyDescent="0.25">
@@ -5011,18 +5038,18 @@
         <v>46</v>
       </c>
       <c r="D54" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E54" t="s">
         <v>27</v>
       </c>
       <c r="F54" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="55" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="56" spans="2:8" x14ac:dyDescent="0.25">
@@ -5030,13 +5057,13 @@
         <v>57</v>
       </c>
       <c r="D56" t="s">
+        <v>157</v>
+      </c>
+      <c r="E56" t="s">
+        <v>27</v>
+      </c>
+      <c r="F56" t="s">
         <v>159</v>
-      </c>
-      <c r="E56" t="s">
-        <v>27</v>
-      </c>
-      <c r="F56" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="58" spans="2:8" x14ac:dyDescent="0.25">
@@ -5049,13 +5076,13 @@
         <v>55</v>
       </c>
       <c r="D59" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E59" t="s">
         <v>27</v>
       </c>
       <c r="F59" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="60" spans="2:8" x14ac:dyDescent="0.25">
@@ -5063,46 +5090,46 @@
         <v>56</v>
       </c>
       <c r="D60" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E60" t="s">
         <v>27</v>
       </c>
       <c r="F60" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="61" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C61" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D61" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E61" t="s">
         <v>27</v>
       </c>
       <c r="F61" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="G61" s="60"/>
     </row>
     <row r="62" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C62" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D62" t="s">
+        <v>145</v>
+      </c>
+      <c r="E62" t="s">
+        <v>27</v>
+      </c>
+      <c r="F62" t="s">
         <v>147</v>
-      </c>
-      <c r="E62" t="s">
-        <v>27</v>
-      </c>
-      <c r="F62" t="s">
-        <v>149</v>
       </c>
       <c r="G62" s="60"/>
       <c r="H62" s="45" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="63" spans="2:8" x14ac:dyDescent="0.25">
@@ -5110,13 +5137,13 @@
         <v>47</v>
       </c>
       <c r="D63" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E63" t="s">
         <v>27</v>
       </c>
       <c r="F63" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="64" spans="2:8" x14ac:dyDescent="0.25">
@@ -5124,13 +5151,13 @@
         <v>48</v>
       </c>
       <c r="D64" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E64" t="s">
         <v>27</v>
       </c>
       <c r="F64" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
@@ -5138,13 +5165,13 @@
         <v>49</v>
       </c>
       <c r="D65" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E65" t="s">
         <v>27</v>
       </c>
       <c r="F65" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
@@ -5152,13 +5179,13 @@
         <v>50</v>
       </c>
       <c r="D66" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E66" t="s">
         <v>27</v>
       </c>
       <c r="F66" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
@@ -5166,36 +5193,36 @@
         <v>51</v>
       </c>
       <c r="D67" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E67" t="s">
         <v>27</v>
       </c>
       <c r="F67" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C68" s="64" t="s">
+      <c r="C68" s="65" t="s">
         <v>52</v>
       </c>
       <c r="D68" t="s">
-        <v>134</v>
-      </c>
-      <c r="E68" s="64" t="s">
-        <v>27</v>
-      </c>
-      <c r="F68" s="64" t="s">
-        <v>172</v>
+        <v>132</v>
+      </c>
+      <c r="E68" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="F68" s="65" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C69" s="64"/>
+      <c r="C69" s="65"/>
       <c r="D69" t="s">
-        <v>128</v>
-      </c>
-      <c r="E69" s="64"/>
-      <c r="F69" s="64"/>
+        <v>126</v>
+      </c>
+      <c r="E69" s="65"/>
+      <c r="F69" s="65"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
@@ -5204,16 +5231,16 @@
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C72" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D72" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E72" t="s">
         <v>27</v>
       </c>
       <c r="F72" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
@@ -5221,13 +5248,13 @@
         <v>54</v>
       </c>
       <c r="D73" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E73" t="s">
         <v>27</v>
       </c>
       <c r="F73" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
@@ -5237,12 +5264,12 @@
       <c r="A75" s="18"/>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C76" s="64"/>
-      <c r="F76" s="64"/>
+      <c r="C76" s="65"/>
+      <c r="F76" s="65"/>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C77" s="64"/>
-      <c r="F77" s="64"/>
+      <c r="C77" s="65"/>
+      <c r="F77" s="65"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>